<commit_message>
Adds output data for fixed code
</commit_message>
<xml_diff>
--- a/Data/output_results.xlsx
+++ b/Data/output_results.xlsx
@@ -70,13 +70,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D170"/>
+  <dimension ref="A1:D274"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.51171875" customWidth="true"/>
     <col min="2" max="2" width="3.64453125" customWidth="true"/>
-    <col min="3" max="3" width="12.24609375" customWidth="true"/>
-    <col min="4" max="4" width="13.24609375" customWidth="true"/>
+    <col min="3" max="3" width="12.64453125" customWidth="true"/>
+    <col min="4" max="4" width="12.64453125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -101,10 +101,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="0">
-        <v>0</v>
+        <v>0.56913666422259146</v>
       </c>
       <c r="D2" s="0">
-        <v>0</v>
+        <v>0.35256802490180772</v>
       </c>
     </row>
     <row r="3">
@@ -115,10 +115,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="0">
-        <v>0</v>
+        <v>0.73225779953392556</v>
       </c>
       <c r="D3" s="0">
-        <v>0</v>
+        <v>0.45361808916891094</v>
       </c>
     </row>
     <row r="4">
@@ -129,10 +129,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="0">
-        <v>0</v>
+        <v>0.7222329673233292</v>
       </c>
       <c r="D4" s="0">
-        <v>0</v>
+        <v>0.44740791942472508</v>
       </c>
     </row>
     <row r="5">
@@ -143,10 +143,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="0">
-        <v>0</v>
+        <v>0.70787166825538173</v>
       </c>
       <c r="D5" s="0">
-        <v>0</v>
+        <v>0.43851140095085972</v>
       </c>
     </row>
     <row r="6">
@@ -157,10 +157,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="0">
-        <v>0</v>
+        <v>0.69199975814718229</v>
       </c>
       <c r="D6" s="0">
-        <v>0</v>
+        <v>0.42867909115596953</v>
       </c>
     </row>
     <row r="7">
@@ -171,10 +171,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="0">
-        <v>0</v>
+        <v>0.67590259958445376</v>
       </c>
       <c r="D7" s="0">
-        <v>0</v>
+        <v>0.41870724474761234</v>
       </c>
     </row>
     <row r="8">
@@ -185,10 +185,10 @@
         <v>3</v>
       </c>
       <c r="C8" s="0">
-        <v>0</v>
+        <v>0.65995720776818412</v>
       </c>
       <c r="D8" s="0">
-        <v>0</v>
+        <v>0.40882941460179539</v>
       </c>
     </row>
     <row r="9">
@@ -199,10 +199,10 @@
         <v>3</v>
       </c>
       <c r="C9" s="0">
-        <v>0</v>
+        <v>0.64363396512439819</v>
       </c>
       <c r="D9" s="0">
-        <v>0</v>
+        <v>0.39871751392715926</v>
       </c>
     </row>
     <row r="10">
@@ -213,10 +213,10 @@
         <v>3</v>
       </c>
       <c r="C10" s="0">
-        <v>1.5462192508980543</v>
+        <v>0.65225074948772299</v>
       </c>
       <c r="D10" s="0">
-        <v>0.95784984806578999</v>
+        <v>0.40405542806089717</v>
       </c>
     </row>
     <row r="11">
@@ -227,10 +227,10 @@
         <v>3</v>
       </c>
       <c r="C11" s="0">
-        <v>0</v>
+        <v>0.63606044591758182</v>
       </c>
       <c r="D11" s="0">
-        <v>0</v>
+        <v>0.39402588030705071</v>
       </c>
     </row>
     <row r="12">
@@ -241,10 +241,10 @@
         <v>3</v>
       </c>
       <c r="C12" s="0">
-        <v>0</v>
+        <v>0.61977519286289107</v>
       </c>
       <c r="D12" s="0">
-        <v>0</v>
+        <v>0.38393751337261461</v>
       </c>
     </row>
     <row r="13">
@@ -255,10 +255,10 @@
         <v>3</v>
       </c>
       <c r="C13" s="0">
-        <v>0</v>
+        <v>0.60326509852836563</v>
       </c>
       <c r="D13" s="0">
-        <v>0</v>
+        <v>0.37370986206075046</v>
       </c>
     </row>
     <row r="14">
@@ -269,10 +269,10 @@
         <v>3</v>
       </c>
       <c r="C14" s="0">
-        <v>0</v>
+        <v>0.58632543032555662</v>
       </c>
       <c r="D14" s="0">
-        <v>0</v>
+        <v>0.36321609889946432</v>
       </c>
     </row>
     <row r="15">
@@ -283,10 +283,10 @@
         <v>3.1000000000000001</v>
       </c>
       <c r="C15" s="0">
-        <v>0</v>
+        <v>0.62796853199463776</v>
       </c>
       <c r="D15" s="0">
-        <v>0</v>
+        <v>0.35256802490180766</v>
       </c>
     </row>
     <row r="16">
@@ -297,10 +297,10 @@
         <v>3.1000000000000001</v>
       </c>
       <c r="C16" s="0">
-        <v>0</v>
+        <v>0.80795155947833952</v>
       </c>
       <c r="D16" s="0">
-        <v>0</v>
+        <v>0.45361808916891067</v>
       </c>
     </row>
     <row r="17">
@@ -311,10 +311,10 @@
         <v>3.1000000000000001</v>
       </c>
       <c r="C17" s="0">
-        <v>0</v>
+        <v>0.79689045664923308</v>
       </c>
       <c r="D17" s="0">
-        <v>0</v>
+        <v>0.44740791942472491</v>
       </c>
     </row>
     <row r="18">
@@ -325,10 +325,10 @@
         <v>3.1000000000000001</v>
       </c>
       <c r="C18" s="0">
-        <v>0</v>
+        <v>0.78104462477763237</v>
       </c>
       <c r="D18" s="0">
-        <v>0</v>
+        <v>0.43851140095085961</v>
       </c>
     </row>
     <row r="19">
@@ -339,10 +339,10 @@
         <v>3.1000000000000001</v>
       </c>
       <c r="C19" s="0">
-        <v>0</v>
+        <v>0.76353202944306309</v>
       </c>
       <c r="D19" s="0">
-        <v>0</v>
+        <v>0.42867909115596936</v>
       </c>
     </row>
     <row r="20">
@@ -353,10 +353,10 @@
         <v>3.1000000000000001</v>
       </c>
       <c r="C20" s="0">
-        <v>0</v>
+        <v>0.74577090163779469</v>
       </c>
       <c r="D20" s="0">
-        <v>0</v>
+        <v>0.41870724474761223</v>
       </c>
     </row>
     <row r="21">
@@ -367,10 +367,10 @@
         <v>3.1000000000000001</v>
       </c>
       <c r="C21" s="0">
-        <v>0</v>
+        <v>0.72817722876377655</v>
       </c>
       <c r="D21" s="0">
-        <v>0</v>
+        <v>0.40882941460179517</v>
       </c>
     </row>
     <row r="22">
@@ -381,10 +381,10 @@
         <v>3.1000000000000001</v>
       </c>
       <c r="C22" s="0">
-        <v>0</v>
+        <v>0.71016664648225702</v>
       </c>
       <c r="D22" s="0">
-        <v>0</v>
+        <v>0.3987175139271591</v>
       </c>
     </row>
     <row r="23">
@@ -395,10 +395,10 @@
         <v>3.1000000000000001</v>
       </c>
       <c r="C23" s="0">
-        <v>0</v>
+        <v>0.71967415103662047</v>
       </c>
       <c r="D23" s="0">
-        <v>0</v>
+        <v>0.40405542806089706</v>
       </c>
     </row>
     <row r="24">
@@ -409,10 +409,10 @@
         <v>3.1000000000000001</v>
       </c>
       <c r="C24" s="0">
-        <v>0</v>
+        <v>0.70181024979002493</v>
       </c>
       <c r="D24" s="0">
-        <v>0</v>
+        <v>0.39402588030705049</v>
       </c>
     </row>
     <row r="25">
@@ -423,10 +423,10 @@
         <v>3.1000000000000001</v>
       </c>
       <c r="C25" s="0">
-        <v>0</v>
+        <v>0.68384158409549556</v>
       </c>
       <c r="D25" s="0">
-        <v>0</v>
+        <v>0.38393751337261439</v>
       </c>
     </row>
     <row r="26">
@@ -437,10 +437,10 @@
         <v>3.1000000000000001</v>
       </c>
       <c r="C26" s="0">
-        <v>0</v>
+        <v>0.66562483519476057</v>
       </c>
       <c r="D26" s="0">
-        <v>0</v>
+        <v>0.3737098620607503</v>
       </c>
     </row>
     <row r="27">
@@ -451,10 +451,10 @@
         <v>3.1000000000000001</v>
       </c>
       <c r="C27" s="0">
-        <v>0</v>
+        <v>0.64693410721587596</v>
       </c>
       <c r="D27" s="0">
-        <v>0</v>
+        <v>0.36321609889946416</v>
       </c>
     </row>
     <row r="28">
@@ -465,10 +465,10 @@
         <v>3.2000000000000002</v>
       </c>
       <c r="C28" s="0">
-        <v>0</v>
+        <v>0.69072111900910649</v>
       </c>
       <c r="D28" s="0">
-        <v>0</v>
+        <v>0.35256802490180766</v>
       </c>
     </row>
     <row r="29">
@@ -479,10 +479,10 @@
         <v>3.2000000000000002</v>
       </c>
       <c r="C29" s="0">
-        <v>0</v>
+        <v>0.88868976204176531</v>
       </c>
       <c r="D29" s="0">
-        <v>0</v>
+        <v>0.45361808916891067</v>
       </c>
     </row>
     <row r="30">
@@ -493,10 +493,10 @@
         <v>3.2000000000000002</v>
       </c>
       <c r="C30" s="0">
-        <v>0</v>
+        <v>0.87652332863892024</v>
       </c>
       <c r="D30" s="0">
-        <v>0</v>
+        <v>0.44740791942472491</v>
       </c>
     </row>
     <row r="31">
@@ -507,10 +507,10 @@
         <v>3.2000000000000002</v>
       </c>
       <c r="C31" s="0">
-        <v>0</v>
+        <v>0.85909403057008704</v>
       </c>
       <c r="D31" s="0">
-        <v>0</v>
+        <v>0.43851140095085966</v>
       </c>
     </row>
     <row r="32">
@@ -521,10 +521,10 @@
         <v>3.2000000000000002</v>
       </c>
       <c r="C32" s="0">
-        <v>0</v>
+        <v>0.8398314101839579</v>
       </c>
       <c r="D32" s="0">
-        <v>0</v>
+        <v>0.42867909115596931</v>
       </c>
     </row>
     <row r="33">
@@ -535,10 +535,10 @@
         <v>3.2000000000000002</v>
       </c>
       <c r="C33" s="0">
-        <v>0</v>
+        <v>0.82029542159938407</v>
       </c>
       <c r="D33" s="0">
-        <v>0</v>
+        <v>0.41870724474761206</v>
       </c>
     </row>
     <row r="34">
@@ -549,10 +549,10 @@
         <v>3.2000000000000002</v>
       </c>
       <c r="C34" s="0">
-        <v>0</v>
+        <v>0.80094362163510546</v>
       </c>
       <c r="D34" s="0">
-        <v>0</v>
+        <v>0.40882941460179512</v>
       </c>
     </row>
     <row r="35">
@@ -563,10 +563,10 @@
         <v>3.2000000000000002</v>
       </c>
       <c r="C35" s="0">
-        <v>0</v>
+        <v>0.78113325071097306</v>
       </c>
       <c r="D35" s="0">
-        <v>0</v>
+        <v>0.39871751392715904</v>
       </c>
     </row>
     <row r="36">
@@ -577,10 +577,10 @@
         <v>3.2000000000000002</v>
       </c>
       <c r="C36" s="0">
-        <v>0</v>
+        <v>0.79159083552643328</v>
       </c>
       <c r="D36" s="0">
-        <v>0</v>
+        <v>0.40405542806089689</v>
       </c>
     </row>
     <row r="37">
@@ -591,10 +591,10 @@
         <v>3.2000000000000002</v>
       </c>
       <c r="C37" s="0">
-        <v>0</v>
+        <v>0.77194180340101171</v>
       </c>
       <c r="D37" s="0">
-        <v>0</v>
+        <v>0.39402588030705055</v>
       </c>
     </row>
     <row r="38">
@@ -605,10 +605,10 @@
         <v>3.2000000000000002</v>
       </c>
       <c r="C38" s="0">
-        <v>0</v>
+        <v>0.75217753776782237</v>
       </c>
       <c r="D38" s="0">
-        <v>0</v>
+        <v>0.38393751337261434</v>
       </c>
     </row>
     <row r="39">
@@ -619,10 +619,10 @@
         <v>3.2000000000000002</v>
       </c>
       <c r="C39" s="0">
-        <v>0</v>
+        <v>0.73214039809546227</v>
       </c>
       <c r="D39" s="0">
-        <v>0</v>
+        <v>0.37370986206075035</v>
       </c>
     </row>
     <row r="40">
@@ -633,10 +633,10 @@
         <v>3.2000000000000002</v>
       </c>
       <c r="C40" s="0">
-        <v>0</v>
+        <v>0.71158191484843836</v>
       </c>
       <c r="D40" s="0">
-        <v>0</v>
+        <v>0.36321609889946416</v>
       </c>
     </row>
     <row r="41">
@@ -647,10 +647,10 @@
         <v>3.2999999999999998</v>
       </c>
       <c r="C41" s="0">
-        <v>0</v>
+        <v>0.75752090008026896</v>
       </c>
       <c r="D41" s="0">
-        <v>0</v>
+        <v>0.35256802490180761</v>
       </c>
     </row>
     <row r="42">
@@ -661,10 +661,10 @@
         <v>3.2999999999999998</v>
       </c>
       <c r="C42" s="0">
-        <v>0</v>
+        <v>0.97463513117965439</v>
       </c>
       <c r="D42" s="0">
-        <v>0</v>
+        <v>0.45361808916891067</v>
       </c>
     </row>
     <row r="43">
@@ -675,10 +675,10 @@
         <v>3.2999999999999998</v>
       </c>
       <c r="C43" s="0">
-        <v>0</v>
+        <v>0.96129207950735063</v>
       </c>
       <c r="D43" s="0">
-        <v>0</v>
+        <v>0.44740791942472485</v>
       </c>
     </row>
     <row r="44">
@@ -689,10 +689,10 @@
         <v>3.2999999999999998</v>
       </c>
       <c r="C44" s="0">
-        <v>0</v>
+        <v>0.94217719044791282</v>
       </c>
       <c r="D44" s="0">
-        <v>0</v>
+        <v>0.43851140095085961</v>
       </c>
     </row>
     <row r="45">
@@ -703,10 +703,10 @@
         <v>3.2999999999999998</v>
       </c>
       <c r="C45" s="0">
-        <v>0</v>
+        <v>0.92105167809389932</v>
       </c>
       <c r="D45" s="0">
-        <v>0</v>
+        <v>0.42867909115596936</v>
       </c>
     </row>
     <row r="46">
@@ -717,10 +717,10 @@
         <v>3.2999999999999998</v>
       </c>
       <c r="C46" s="0">
-        <v>0</v>
+        <v>0.89962636004690755</v>
       </c>
       <c r="D46" s="0">
-        <v>0</v>
+        <v>0.41870724474761217</v>
       </c>
     </row>
     <row r="47">
@@ -731,10 +731,10 @@
         <v>3.2999999999999998</v>
       </c>
       <c r="C47" s="0">
-        <v>0</v>
+        <v>0.87840304353945275</v>
       </c>
       <c r="D47" s="0">
-        <v>0</v>
+        <v>0.40882941460179523</v>
       </c>
     </row>
     <row r="48">
@@ -745,10 +745,10 @@
         <v>3.2999999999999998</v>
       </c>
       <c r="C48" s="0">
-        <v>0</v>
+        <v>0.85667680758057363</v>
       </c>
       <c r="D48" s="0">
-        <v>0</v>
+        <v>0.3987175139271591</v>
       </c>
     </row>
     <row r="49">
@@ -759,10 +759,10 @@
         <v>3.2999999999999998</v>
       </c>
       <c r="C49" s="0">
-        <v>0</v>
+        <v>0.86814574756815899</v>
       </c>
       <c r="D49" s="0">
-        <v>0</v>
+        <v>0.404055428060897</v>
       </c>
     </row>
     <row r="50">
@@ -773,10 +773,10 @@
         <v>3.2999999999999998</v>
       </c>
       <c r="C50" s="0">
-        <v>0</v>
+        <v>0.84659645351630131</v>
       </c>
       <c r="D50" s="0">
-        <v>0</v>
+        <v>0.39402588030705066</v>
       </c>
     </row>
     <row r="51">
@@ -787,10 +787,10 @@
         <v>3.2999999999999998</v>
       </c>
       <c r="C51" s="0">
-        <v>0</v>
+        <v>0.82492078170050753</v>
       </c>
       <c r="D51" s="0">
-        <v>0</v>
+        <v>0.38393751337261439</v>
       </c>
     </row>
     <row r="52">
@@ -801,10 +801,10 @@
         <v>3.2999999999999998</v>
       </c>
       <c r="C52" s="0">
-        <v>0</v>
+        <v>0.80294584614125442</v>
       </c>
       <c r="D52" s="0">
-        <v>0</v>
+        <v>0.37370986206075035</v>
       </c>
     </row>
     <row r="53">
@@ -815,10 +815,10 @@
         <v>3.2999999999999998</v>
       </c>
       <c r="C53" s="0">
-        <v>0</v>
+        <v>0.78039914776331543</v>
       </c>
       <c r="D53" s="0">
-        <v>0</v>
+        <v>0.3632160988994641</v>
       </c>
     </row>
     <row r="54">
@@ -829,10 +829,10 @@
         <v>3.3999999999999999</v>
       </c>
       <c r="C54" s="0">
-        <v>0</v>
+        <v>0.82849435002239713</v>
       </c>
       <c r="D54" s="0">
-        <v>0</v>
+        <v>0.35256802490180755</v>
       </c>
     </row>
     <row r="55">
@@ -843,10 +843,10 @@
         <v>3.3999999999999999</v>
       </c>
       <c r="C55" s="0">
-        <v>0</v>
+        <v>1.0659503908474592</v>
       </c>
       <c r="D55" s="0">
-        <v>0</v>
+        <v>0.45361808916891078</v>
       </c>
     </row>
     <row r="56">
@@ -857,10 +857,10 @@
         <v>3.3999999999999999</v>
       </c>
       <c r="C56" s="0">
-        <v>0</v>
+        <v>1.0513572054694857</v>
       </c>
       <c r="D56" s="0">
-        <v>0</v>
+        <v>0.44740791942472491</v>
       </c>
     </row>
     <row r="57">
@@ -871,10 +871,10 @@
         <v>3.3999999999999999</v>
       </c>
       <c r="C57" s="0">
-        <v>0</v>
+        <v>1.0304514092262784</v>
       </c>
       <c r="D57" s="0">
-        <v>0</v>
+        <v>0.43851140095085966</v>
       </c>
     </row>
     <row r="58">
@@ -885,10 +885,10 @@
         <v>3.3999999999999999</v>
       </c>
       <c r="C58" s="0">
-        <v>0</v>
+        <v>1.0073466108969198</v>
       </c>
       <c r="D58" s="0">
-        <v>0</v>
+        <v>0.42867909115596925</v>
       </c>
     </row>
     <row r="59">
@@ -899,10 +899,10 @@
         <v>3.3999999999999999</v>
       </c>
       <c r="C59" s="0">
-        <v>0</v>
+        <v>0.98391391755805047</v>
       </c>
       <c r="D59" s="0">
-        <v>0</v>
+        <v>0.41870724474761228</v>
       </c>
     </row>
     <row r="60">
@@ -913,10 +913,10 @@
         <v>3.3999999999999999</v>
       </c>
       <c r="C60" s="0">
-        <v>0</v>
+        <v>0.9607021516341</v>
       </c>
       <c r="D60" s="0">
-        <v>0</v>
+        <v>0.40882941460179528</v>
       </c>
     </row>
     <row r="61">
@@ -927,10 +927,10 @@
         <v>3.3999999999999999</v>
       </c>
       <c r="C61" s="0">
-        <v>0</v>
+        <v>0.93694034686108651</v>
       </c>
       <c r="D61" s="0">
-        <v>0</v>
+        <v>0.39871751392715915</v>
       </c>
     </row>
     <row r="62">
@@ -941,10 +941,10 @@
         <v>3.3999999999999999</v>
       </c>
       <c r="C62" s="0">
-        <v>0</v>
+        <v>0.94948383177279472</v>
       </c>
       <c r="D62" s="0">
-        <v>0</v>
+        <v>0.40405542806089706</v>
       </c>
     </row>
     <row r="63">
@@ -955,10 +955,10 @@
         <v>3.3999999999999999</v>
       </c>
       <c r="C63" s="0">
-        <v>0</v>
+        <v>0.92591554690165301</v>
       </c>
       <c r="D63" s="0">
-        <v>0</v>
+        <v>0.39402588030705066</v>
       </c>
     </row>
     <row r="64">
@@ -969,10 +969,10 @@
         <v>3.3999999999999999</v>
       </c>
       <c r="C64" s="0">
-        <v>0</v>
+        <v>0.90220904371418731</v>
       </c>
       <c r="D64" s="0">
-        <v>0</v>
+        <v>0.38393751337261439</v>
       </c>
     </row>
     <row r="65">
@@ -983,10 +983,10 @@
         <v>3.3999999999999999</v>
       </c>
       <c r="C65" s="0">
-        <v>0</v>
+        <v>0.87817523824292121</v>
       </c>
       <c r="D65" s="0">
-        <v>0</v>
+        <v>0.37370986206075035</v>
       </c>
     </row>
     <row r="66">
@@ -997,10 +997,10 @@
         <v>3.3999999999999999</v>
       </c>
       <c r="C66" s="0">
-        <v>0</v>
+        <v>0.85351610050058035</v>
       </c>
       <c r="D66" s="0">
-        <v>0</v>
+        <v>0.36321609889946421</v>
       </c>
     </row>
     <row r="67">
@@ -1011,10 +1011,10 @@
         <v>3.5</v>
       </c>
       <c r="C67" s="0">
-        <v>0</v>
+        <v>0.90376794364976321</v>
       </c>
       <c r="D67" s="0">
-        <v>0</v>
+        <v>0.35256802490180772</v>
       </c>
     </row>
     <row r="68">
@@ -1025,10 +1025,10 @@
         <v>3.5</v>
       </c>
       <c r="C68" s="0">
-        <v>0</v>
+        <v>1.1627982650006314</v>
       </c>
       <c r="D68" s="0">
-        <v>0</v>
+        <v>0.45361808916891083</v>
       </c>
     </row>
     <row r="69">
@@ -1039,10 +1039,10 @@
         <v>3.5</v>
       </c>
       <c r="C69" s="0">
-        <v>0</v>
+        <v>1.1468792027402863</v>
       </c>
       <c r="D69" s="0">
-        <v>0</v>
+        <v>0.44740791942472502</v>
       </c>
     </row>
     <row r="70">
@@ -1053,10 +1053,10 @@
         <v>3.5</v>
       </c>
       <c r="C70" s="0">
-        <v>0</v>
+        <v>1.1240739917203513</v>
       </c>
       <c r="D70" s="0">
-        <v>0</v>
+        <v>0.43851140095085961</v>
       </c>
     </row>
     <row r="71">
@@ -1067,10 +1067,10 @@
         <v>3.5</v>
       </c>
       <c r="C71" s="0">
-        <v>0</v>
+        <v>1.098869986317053</v>
       </c>
       <c r="D71" s="0">
-        <v>0</v>
+        <v>0.42867909115596942</v>
       </c>
     </row>
     <row r="72">
@@ -1081,10 +1081,10 @@
         <v>3.5</v>
       </c>
       <c r="C72" s="0">
-        <v>0</v>
+        <v>1.0733082947104979</v>
       </c>
       <c r="D72" s="0">
-        <v>0</v>
+        <v>0.41870724474761223</v>
       </c>
     </row>
     <row r="73">
@@ -1095,10 +1095,10 @@
         <v>3.5</v>
       </c>
       <c r="C73" s="0">
-        <v>0</v>
+        <v>1.0479876030763291</v>
       </c>
       <c r="D73" s="0">
-        <v>0</v>
+        <v>0.40882941460179528</v>
       </c>
     </row>
     <row r="74">
@@ -1109,10 +1109,10 @@
         <v>3.5</v>
       </c>
       <c r="C74" s="0">
-        <v>0</v>
+        <v>1.0220668983225392</v>
       </c>
       <c r="D74" s="0">
-        <v>0</v>
+        <v>0.3987175139271591</v>
       </c>
     </row>
     <row r="75">
@@ -1123,10 +1123,10 @@
         <v>3.5</v>
       </c>
       <c r="C75" s="0">
-        <v>0</v>
+        <v>1.0357500327513376</v>
       </c>
       <c r="D75" s="0">
-        <v>0</v>
+        <v>0.40405542806089706</v>
       </c>
     </row>
     <row r="76">
@@ -1137,10 +1137,10 @@
         <v>3.5</v>
       </c>
       <c r="C76" s="0">
-        <v>0</v>
+        <v>1.0100404303228265</v>
       </c>
       <c r="D76" s="0">
-        <v>0</v>
+        <v>0.39402588030705066</v>
       </c>
     </row>
     <row r="77">
@@ -1151,10 +1151,10 @@
         <v>3.5</v>
       </c>
       <c r="C77" s="0">
-        <v>0</v>
+        <v>0.98418005162949795</v>
       </c>
       <c r="D77" s="0">
-        <v>0</v>
+        <v>0.3839375133726145</v>
       </c>
     </row>
     <row r="78">
@@ -1165,10 +1165,10 @@
         <v>3.5</v>
       </c>
       <c r="C78" s="0">
-        <v>0</v>
+        <v>0.95796263331124709</v>
       </c>
       <c r="D78" s="0">
-        <v>0</v>
+        <v>0.37370986206075041</v>
       </c>
     </row>
     <row r="79">
@@ -1179,10 +1179,10 @@
         <v>3.5</v>
       </c>
       <c r="C79" s="0">
-        <v>0</v>
+        <v>0.93106306760030477</v>
       </c>
       <c r="D79" s="0">
-        <v>0</v>
+        <v>0.36321609889946416</v>
       </c>
     </row>
     <row r="80">
@@ -1193,10 +1193,10 @@
         <v>3.6000000000000001</v>
       </c>
       <c r="C80" s="0">
-        <v>0</v>
+        <v>0.9834681557766376</v>
       </c>
       <c r="D80" s="0">
-        <v>0</v>
+        <v>0.3525680249018075</v>
       </c>
     </row>
     <row r="81">
@@ -1207,10 +1207,10 @@
         <v>3.6000000000000001</v>
       </c>
       <c r="C81" s="0">
-        <v>0</v>
+        <v>1.2653414775946232</v>
       </c>
       <c r="D81" s="0">
-        <v>0</v>
+        <v>0.45361808916891078</v>
       </c>
     </row>
     <row r="82">
@@ -1221,10 +1221,10 @@
         <v>3.6000000000000001</v>
       </c>
       <c r="C82" s="0">
-        <v>0</v>
+        <v>1.2480185675347124</v>
       </c>
       <c r="D82" s="0">
-        <v>0</v>
+        <v>0.44740791942472485</v>
       </c>
     </row>
     <row r="83">
@@ -1235,10 +1235,10 @@
         <v>3.6000000000000001</v>
       </c>
       <c r="C83" s="0">
-        <v>0</v>
+        <v>1.2232022427452993</v>
       </c>
       <c r="D83" s="0">
-        <v>0</v>
+        <v>0.4385114009508595</v>
       </c>
     </row>
     <row r="84">
@@ -1249,10 +1249,10 @@
         <v>3.6000000000000001</v>
       </c>
       <c r="C84" s="0">
-        <v>0</v>
+        <v>1.1957755820783305</v>
       </c>
       <c r="D84" s="0">
-        <v>0</v>
+        <v>0.42867909115596925</v>
       </c>
     </row>
     <row r="85">
@@ -1263,10 +1263,10 @@
         <v>3.6000000000000001</v>
       </c>
       <c r="C85" s="0">
-        <v>0</v>
+        <v>1.1679596920819357</v>
       </c>
       <c r="D85" s="0">
-        <v>0</v>
+        <v>0.41870724474761217</v>
       </c>
     </row>
     <row r="86">
@@ -1277,10 +1277,10 @@
         <v>3.6000000000000001</v>
       </c>
       <c r="C86" s="0">
-        <v>0</v>
+        <v>1.1404060550234221</v>
       </c>
       <c r="D86" s="0">
-        <v>0</v>
+        <v>0.40882941460179528</v>
       </c>
     </row>
     <row r="87">
@@ -1291,10 +1291,10 @@
         <v>3.6000000000000001</v>
       </c>
       <c r="C87" s="0">
-        <v>0</v>
+        <v>1.1121994917349598</v>
       </c>
       <c r="D87" s="0">
-        <v>0</v>
+        <v>0.3987175139271591</v>
       </c>
     </row>
     <row r="88">
@@ -1305,10 +1305,10 @@
         <v>3.6000000000000001</v>
       </c>
       <c r="C88" s="0">
-        <v>0</v>
+        <v>1.1270892951147851</v>
       </c>
       <c r="D88" s="0">
-        <v>0</v>
+        <v>0.404055428060897</v>
       </c>
     </row>
     <row r="89">
@@ -1319,10 +1319,10 @@
         <v>3.6000000000000001</v>
       </c>
       <c r="C89" s="0">
-        <v>0</v>
+        <v>1.0991124505455814</v>
       </c>
       <c r="D89" s="0">
-        <v>0</v>
+        <v>0.3940258803070506</v>
       </c>
     </row>
     <row r="90">
@@ -1333,10 +1333,10 @@
         <v>3.6000000000000001</v>
       </c>
       <c r="C90" s="0">
-        <v>0</v>
+        <v>1.0709715332670755</v>
       </c>
       <c r="D90" s="0">
-        <v>0</v>
+        <v>0.38393751337261445</v>
       </c>
     </row>
     <row r="91">
@@ -1347,10 +1347,10 @@
         <v>3.6000000000000001</v>
       </c>
       <c r="C91" s="0">
-        <v>0</v>
+        <v>1.0424420902570155</v>
       </c>
       <c r="D91" s="0">
-        <v>0</v>
+        <v>0.3737098620607503</v>
       </c>
     </row>
     <row r="92">
@@ -1361,10 +1361,10 @@
         <v>3.6000000000000001</v>
       </c>
       <c r="C92" s="0">
-        <v>0</v>
+        <v>1.0131703436025616</v>
       </c>
       <c r="D92" s="0">
-        <v>0</v>
+        <v>0.36321609889946416</v>
       </c>
     </row>
     <row r="93">
@@ -1375,10 +1375,10 @@
         <v>3.7000000000000002</v>
       </c>
       <c r="C93" s="0">
-        <v>0</v>
+        <v>1.0677214612172932</v>
       </c>
       <c r="D93" s="0">
-        <v>0</v>
+        <v>0.35256802490180761</v>
       </c>
     </row>
     <row r="94">
@@ -1389,10 +1389,10 @@
         <v>3.7000000000000002</v>
       </c>
       <c r="C94" s="0">
-        <v>0</v>
+        <v>1.373742752584886</v>
       </c>
       <c r="D94" s="0">
-        <v>0</v>
+        <v>0.45361808916891078</v>
       </c>
     </row>
     <row r="95">
@@ -1403,10 +1403,10 @@
         <v>3.7000000000000002</v>
       </c>
       <c r="C95" s="0">
-        <v>0</v>
+        <v>1.3549357960677251</v>
       </c>
       <c r="D95" s="0">
-        <v>0</v>
+        <v>0.44740791942472485</v>
       </c>
     </row>
     <row r="96">
@@ -1417,10 +1417,10 @@
         <v>3.7000000000000002</v>
       </c>
       <c r="C96" s="0">
-        <v>0</v>
+        <v>1.3279934671162907</v>
       </c>
       <c r="D96" s="0">
-        <v>0</v>
+        <v>0.43851140095085966</v>
       </c>
     </row>
     <row r="97">
@@ -1431,10 +1431,10 @@
         <v>3.7000000000000002</v>
       </c>
       <c r="C97" s="0">
-        <v>0</v>
+        <v>1.2982171759047858</v>
       </c>
       <c r="D97" s="0">
-        <v>0</v>
+        <v>0.42867909115596942</v>
       </c>
     </row>
     <row r="98">
@@ -1445,10 +1445,10 @@
         <v>3.7000000000000002</v>
       </c>
       <c r="C98" s="0">
-        <v>0</v>
+        <v>1.2680183102500493</v>
       </c>
       <c r="D98" s="0">
-        <v>0</v>
+        <v>0.41870724474761228</v>
       </c>
     </row>
     <row r="99">
@@ -1459,10 +1459,10 @@
         <v>3.7000000000000002</v>
       </c>
       <c r="C99" s="0">
-        <v>0</v>
+        <v>1.23810416463266</v>
       </c>
       <c r="D99" s="0">
-        <v>0</v>
+        <v>0.40882941460179523</v>
       </c>
     </row>
     <row r="100">
@@ -1473,10 +1473,10 @@
         <v>3.7000000000000002</v>
       </c>
       <c r="C100" s="0">
-        <v>0</v>
+        <v>1.207481156868375</v>
       </c>
       <c r="D100" s="0">
-        <v>0</v>
+        <v>0.39871751392715904</v>
       </c>
     </row>
     <row r="101">
@@ -1487,10 +1487,10 @@
         <v>3.7000000000000002</v>
       </c>
       <c r="C101" s="0">
-        <v>0</v>
+        <v>1.223646563474134</v>
       </c>
       <c r="D101" s="0">
-        <v>0</v>
+        <v>0.40405542806089695</v>
       </c>
     </row>
     <row r="102">
@@ -1501,10 +1501,10 @@
         <v>3.7000000000000002</v>
       </c>
       <c r="C102" s="0">
-        <v>0</v>
+        <v>1.1932729543356764</v>
       </c>
       <c r="D102" s="0">
-        <v>0</v>
+        <v>0.39402588030705055</v>
       </c>
     </row>
     <row r="103">
@@ -1515,10 +1515,10 @@
         <v>3.7000000000000002</v>
       </c>
       <c r="C103" s="0">
-        <v>0</v>
+        <v>1.162721216447556</v>
       </c>
       <c r="D103" s="0">
-        <v>0</v>
+        <v>0.38393751337261445</v>
       </c>
     </row>
     <row r="104">
@@ -1529,10 +1529,10 @@
         <v>3.7000000000000002</v>
       </c>
       <c r="C104" s="0">
-        <v>0</v>
+        <v>1.1317476679910112</v>
       </c>
       <c r="D104" s="0">
-        <v>0</v>
+        <v>0.37370986206075046</v>
       </c>
     </row>
     <row r="105">
@@ -1543,10 +1543,10 @@
         <v>3.7000000000000002</v>
       </c>
       <c r="C105" s="0">
-        <v>0</v>
+        <v>1.0999682230474226</v>
       </c>
       <c r="D105" s="0">
-        <v>0</v>
+        <v>0.36321609889946416</v>
       </c>
     </row>
     <row r="106">
@@ -1557,10 +1557,10 @@
         <v>3.7999999999999998</v>
       </c>
       <c r="C106" s="0">
-        <v>0</v>
+        <v>1.156654334786001</v>
       </c>
       <c r="D106" s="0">
-        <v>0</v>
+        <v>0.35256802490180766</v>
       </c>
     </row>
     <row r="107">
@@ -1571,10 +1571,10 @@
         <v>3.7999999999999998</v>
       </c>
       <c r="C107" s="0">
-        <v>0</v>
+        <v>1.4881648139268726</v>
       </c>
       <c r="D107" s="0">
-        <v>0</v>
+        <v>0.45361808916891094</v>
       </c>
     </row>
     <row r="108">
@@ -1585,10 +1585,10 @@
         <v>3.7999999999999998</v>
       </c>
       <c r="C108" s="0">
-        <v>0</v>
+        <v>1.4677913845542852</v>
       </c>
       <c r="D108" s="0">
-        <v>0</v>
+        <v>0.44740791942472496</v>
       </c>
     </row>
     <row r="109">
@@ -1599,10 +1599,10 @@
         <v>3.7999999999999998</v>
       </c>
       <c r="C109" s="0">
-        <v>0</v>
+        <v>1.4386049696484924</v>
       </c>
       <c r="D109" s="0">
-        <v>0</v>
+        <v>0.43851140095085966</v>
       </c>
     </row>
     <row r="110">
@@ -1613,10 +1613,10 @@
         <v>3.7999999999999998</v>
       </c>
       <c r="C110" s="0">
-        <v>0</v>
+        <v>1.406348545520451</v>
       </c>
       <c r="D110" s="0">
-        <v>0</v>
+        <v>0.42867909115596947</v>
       </c>
     </row>
     <row r="111">
@@ -1627,10 +1627,10 @@
         <v>3.7999999999999998</v>
       </c>
       <c r="C111" s="0">
-        <v>0</v>
+        <v>1.3736343497925236</v>
       </c>
       <c r="D111" s="0">
-        <v>0</v>
+        <v>0.41870724474761234</v>
       </c>
     </row>
     <row r="112">
@@ -1641,10 +1641,10 @@
         <v>3.7999999999999998</v>
       </c>
       <c r="C112" s="0">
-        <v>0</v>
+        <v>1.3412285890613254</v>
       </c>
       <c r="D112" s="0">
-        <v>0</v>
+        <v>0.40882941460179528</v>
       </c>
     </row>
     <row r="113">
@@ -1655,10 +1655,10 @@
         <v>3.7999999999999998</v>
       </c>
       <c r="C113" s="0">
-        <v>0</v>
+        <v>1.3080549234928134</v>
       </c>
       <c r="D113" s="0">
-        <v>0</v>
+        <v>0.39871751392715915</v>
       </c>
     </row>
     <row r="114">
@@ -1669,10 +1669,10 @@
         <v>3.7999999999999998</v>
       </c>
       <c r="C114" s="0">
-        <v>0</v>
+        <v>1.3255667824403825</v>
       </c>
       <c r="D114" s="0">
-        <v>0</v>
+        <v>0.40405542806089711</v>
       </c>
     </row>
     <row r="115">
@@ -1683,10 +1683,10 @@
         <v>3.7999999999999998</v>
       </c>
       <c r="C115" s="0">
-        <v>0</v>
+        <v>1.2926632884588718</v>
       </c>
       <c r="D115" s="0">
-        <v>0</v>
+        <v>0.39402588030705066</v>
       </c>
     </row>
     <row r="116">
@@ -1697,10 +1697,10 @@
         <v>3.7999999999999998</v>
       </c>
       <c r="C116" s="0">
-        <v>0</v>
+        <v>1.2595668289915758</v>
       </c>
       <c r="D116" s="0">
-        <v>0</v>
+        <v>0.3839375133726145</v>
       </c>
     </row>
     <row r="117">
@@ -1711,10 +1711,10 @@
         <v>3.7999999999999998</v>
       </c>
       <c r="C117" s="0">
-        <v>0</v>
+        <v>1.2260134254240171</v>
       </c>
       <c r="D117" s="0">
-        <v>0</v>
+        <v>0.37370986206075035</v>
       </c>
     </row>
     <row r="118">
@@ -1725,10 +1725,10 @@
         <v>3.7999999999999998</v>
       </c>
       <c r="C118" s="0">
-        <v>0</v>
+        <v>1.1915870004749602</v>
       </c>
       <c r="D118" s="0">
-        <v>0</v>
+        <v>0.36321609889946416</v>
       </c>
     </row>
     <row r="119">
@@ -1739,10 +1739,10 @@
         <v>3.8999999999999999</v>
       </c>
       <c r="C119" s="0">
-        <v>0</v>
+        <v>1.2503932512970326</v>
       </c>
       <c r="D119" s="0">
-        <v>0</v>
+        <v>0.35256802490180755</v>
       </c>
     </row>
     <row r="120">
@@ -1753,10 +1753,10 @@
         <v>3.8999999999999999</v>
       </c>
       <c r="C120" s="0">
-        <v>0</v>
+        <v>1.6087703855760336</v>
       </c>
       <c r="D120" s="0">
-        <v>0</v>
+        <v>0.45361808916891072</v>
       </c>
     </row>
     <row r="121">
@@ -1767,10 +1767,10 @@
         <v>3.8999999999999999</v>
       </c>
       <c r="C121" s="0">
-        <v>0</v>
+        <v>1.5867458292093535</v>
       </c>
       <c r="D121" s="0">
-        <v>0</v>
+        <v>0.44740791942472491</v>
       </c>
     </row>
     <row r="122">
@@ -1781,10 +1781,10 @@
         <v>3.8999999999999999</v>
       </c>
       <c r="C122" s="0">
-        <v>0</v>
+        <v>1.5551940551570729</v>
       </c>
       <c r="D122" s="0">
-        <v>0</v>
+        <v>0.4385114009508595</v>
       </c>
     </row>
     <row r="123">
@@ -1795,10 +1795,10 @@
         <v>3.8999999999999999</v>
       </c>
       <c r="C123" s="0">
-        <v>0</v>
+        <v>1.5203234686493583</v>
       </c>
       <c r="D123" s="0">
-        <v>0</v>
+        <v>0.42867909115596919</v>
       </c>
     </row>
     <row r="124">
@@ -1809,10 +1809,10 @@
         <v>3.8999999999999999</v>
       </c>
       <c r="C124" s="0">
-        <v>0</v>
+        <v>1.484958011287044</v>
       </c>
       <c r="D124" s="0">
-        <v>0</v>
+        <v>0.41870724474761212</v>
       </c>
     </row>
     <row r="125">
@@ -1823,10 +1823,10 @@
         <v>3.8999999999999999</v>
       </c>
       <c r="C125" s="0">
-        <v>0</v>
+        <v>1.4499259854666999</v>
       </c>
       <c r="D125" s="0">
-        <v>0</v>
+        <v>0.40882941460179523</v>
       </c>
     </row>
     <row r="126">
@@ -1837,10 +1837,10 @@
         <v>3.8999999999999999</v>
       </c>
       <c r="C126" s="0">
-        <v>0</v>
+        <v>1.4140638213783019</v>
       </c>
       <c r="D126" s="0">
-        <v>0</v>
+        <v>0.39871751392715904</v>
       </c>
     </row>
     <row r="127">
@@ -1851,10 +1851,10 @@
         <v>3.8999999999999999</v>
       </c>
       <c r="C127" s="0">
-        <v>0</v>
+        <v>1.4329948966245267</v>
       </c>
       <c r="D127" s="0">
-        <v>0</v>
+        <v>0.404055428060897</v>
       </c>
     </row>
     <row r="128">
@@ -1865,10 +1865,10 @@
         <v>3.8999999999999999</v>
       </c>
       <c r="C128" s="0">
-        <v>0</v>
+        <v>1.3974247996809266</v>
       </c>
       <c r="D128" s="0">
-        <v>0</v>
+        <v>0.39402588030705055</v>
       </c>
     </row>
     <row r="129">
@@ -1879,10 +1879,10 @@
         <v>3.8999999999999999</v>
       </c>
       <c r="C129" s="0">
-        <v>0</v>
+        <v>1.3616460987197707</v>
       </c>
       <c r="D129" s="0">
-        <v>0</v>
+        <v>0.38393751337261434</v>
       </c>
     </row>
     <row r="130">
@@ -1893,10 +1893,10 @@
         <v>3.8999999999999999</v>
       </c>
       <c r="C130" s="0">
-        <v>0</v>
+        <v>1.3253734214668187</v>
       </c>
       <c r="D130" s="0">
-        <v>0</v>
+        <v>0.37370986206075035</v>
       </c>
     </row>
     <row r="131">
@@ -1907,10 +1907,10 @@
         <v>3.8999999999999999</v>
       </c>
       <c r="C131" s="0">
-        <v>0</v>
+        <v>1.2881569704252469</v>
       </c>
       <c r="D131" s="0">
-        <v>0</v>
+        <v>0.36321609889946405</v>
       </c>
     </row>
     <row r="132">
@@ -1921,10 +1921,10 @@
         <v>4</v>
       </c>
       <c r="C132" s="0">
-        <v>0</v>
+        <v>1.3490646855646609</v>
       </c>
       <c r="D132" s="0">
-        <v>0</v>
+        <v>0.35256802490180766</v>
       </c>
     </row>
     <row r="133">
@@ -1935,10 +1935,10 @@
         <v>4</v>
       </c>
       <c r="C133" s="0">
-        <v>0</v>
+        <v>1.7357221914878229</v>
       </c>
       <c r="D133" s="0">
-        <v>0</v>
+        <v>0.45361808916891078</v>
       </c>
     </row>
     <row r="134">
@@ -1949,10 +1949,10 @@
         <v>4</v>
       </c>
       <c r="C134" s="0">
-        <v>0</v>
+        <v>1.7119596262478909</v>
       </c>
       <c r="D134" s="0">
-        <v>0</v>
+        <v>0.44740791942472496</v>
       </c>
     </row>
     <row r="135">
@@ -1963,10 +1963,10 @@
         <v>4</v>
       </c>
       <c r="C135" s="0">
-        <v>0</v>
+        <v>1.6779180284572008</v>
       </c>
       <c r="D135" s="0">
-        <v>0</v>
+        <v>0.43851140095085961</v>
       </c>
     </row>
     <row r="136">
@@ -1977,10 +1977,10 @@
         <v>4</v>
       </c>
       <c r="C136" s="0">
-        <v>0</v>
+        <v>1.6402957230155428</v>
       </c>
       <c r="D136" s="0">
-        <v>0</v>
+        <v>0.42867909115596942</v>
       </c>
     </row>
     <row r="137">
@@ -1991,10 +1991,10 @@
         <v>4</v>
       </c>
       <c r="C137" s="0">
-        <v>0</v>
+        <v>1.6021394953112973</v>
       </c>
       <c r="D137" s="0">
-        <v>0</v>
+        <v>0.41870724474761223</v>
       </c>
     </row>
     <row r="138">
@@ -2005,10 +2005,10 @@
         <v>4</v>
       </c>
       <c r="C138" s="0">
-        <v>0</v>
+        <v>1.5643430110060654</v>
       </c>
       <c r="D138" s="0">
-        <v>0</v>
+        <v>0.40882941460179523</v>
       </c>
     </row>
     <row r="139">
@@ -2019,10 +2019,10 @@
         <v>4</v>
       </c>
       <c r="C139" s="0">
-        <v>0</v>
+        <v>1.5256508802948694</v>
       </c>
       <c r="D139" s="0">
-        <v>0</v>
+        <v>0.39871751392715915</v>
       </c>
     </row>
     <row r="140">
@@ -2033,10 +2033,10 @@
         <v>4</v>
       </c>
       <c r="C140" s="0">
-        <v>0</v>
+        <v>1.5460758506375654</v>
       </c>
       <c r="D140" s="0">
-        <v>0</v>
+        <v>0.40405542806089711</v>
       </c>
     </row>
     <row r="141">
@@ -2047,10 +2047,10 @@
         <v>4</v>
       </c>
       <c r="C141" s="0">
-        <v>0</v>
+        <v>1.5076988347676012</v>
       </c>
       <c r="D141" s="0">
-        <v>0</v>
+        <v>0.39402588030705066</v>
       </c>
     </row>
     <row r="142">
@@ -2061,10 +2061,10 @@
         <v>4</v>
       </c>
       <c r="C142" s="0">
-        <v>0</v>
+        <v>1.4690967534527779</v>
       </c>
       <c r="D142" s="0">
-        <v>0</v>
+        <v>0.38393751337261434</v>
       </c>
     </row>
     <row r="143">
@@ -2075,10 +2075,10 @@
         <v>4</v>
       </c>
       <c r="C143" s="0">
-        <v>0</v>
+        <v>1.4299617150301998</v>
       </c>
       <c r="D143" s="0">
-        <v>0</v>
+        <v>0.37370986206075041</v>
       </c>
     </row>
     <row r="144">
@@ -2089,10 +2089,10 @@
         <v>4</v>
       </c>
       <c r="C144" s="0">
-        <v>0</v>
+        <v>1.3898084274383558</v>
       </c>
       <c r="D144" s="0">
-        <v>0</v>
+        <v>0.36321609889946416</v>
       </c>
     </row>
     <row r="145">
@@ -2103,10 +2103,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="C145" s="0">
-        <v>0</v>
+        <v>1.4527951124031557</v>
       </c>
       <c r="D145" s="0">
-        <v>0</v>
+        <v>0.35256802490180772</v>
       </c>
     </row>
     <row r="146">
@@ -2117,10 +2117,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="C146" s="0">
-        <v>-1.5986023489402736</v>
+        <v>1.8691829556176909</v>
       </c>
       <c r="D146" s="0">
-        <v>-0.38795289711358638</v>
+        <v>0.45361808916891083</v>
       </c>
     </row>
     <row r="147">
@@ -2131,10 +2131,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="C147" s="0">
-        <v>0</v>
+        <v>1.8435932718848567</v>
       </c>
       <c r="D147" s="0">
-        <v>0</v>
+        <v>0.44740791942472491</v>
       </c>
     </row>
     <row r="148">
@@ -2145,10 +2145,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="C148" s="0">
-        <v>0</v>
+        <v>1.8069341943640422</v>
       </c>
       <c r="D148" s="0">
-        <v>0</v>
+        <v>0.43851140095085966</v>
       </c>
     </row>
     <row r="149">
@@ -2159,10 +2159,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="C149" s="0">
-        <v>0</v>
+        <v>1.766419086343034</v>
       </c>
       <c r="D149" s="0">
-        <v>0</v>
+        <v>0.42867909115596942</v>
       </c>
     </row>
     <row r="150">
@@ -2173,10 +2173,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="C150" s="0">
-        <v>0</v>
+        <v>1.7253290024429671</v>
       </c>
       <c r="D150" s="0">
-        <v>0</v>
+        <v>0.41870724474761228</v>
       </c>
     </row>
     <row r="151">
@@ -2187,10 +2187,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="C151" s="0">
-        <v>0</v>
+        <v>1.6846263228367031</v>
       </c>
       <c r="D151" s="0">
-        <v>0</v>
+        <v>0.40882941460179523</v>
       </c>
     </row>
     <row r="152">
@@ -2201,10 +2201,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="C152" s="0">
-        <v>0</v>
+        <v>1.6429591300125415</v>
       </c>
       <c r="D152" s="0">
-        <v>0</v>
+        <v>0.39871751392715915</v>
       </c>
     </row>
     <row r="153">
@@ -2215,10 +2215,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="C153" s="0">
-        <v>0</v>
+        <v>1.6649545890904938</v>
       </c>
       <c r="D153" s="0">
-        <v>0</v>
+        <v>0.40405542806089711</v>
       </c>
     </row>
     <row r="154">
@@ -2229,10 +2229,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="C154" s="0">
-        <v>0</v>
+        <v>1.6236267404846529</v>
       </c>
       <c r="D154" s="0">
-        <v>0</v>
+        <v>0.3940258803070506</v>
       </c>
     </row>
     <row r="155">
@@ -2243,10 +2243,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="C155" s="0">
-        <v>0</v>
+        <v>1.5820565210112325</v>
       </c>
       <c r="D155" s="0">
-        <v>0</v>
+        <v>0.38393751337261439</v>
       </c>
     </row>
     <row r="156">
@@ -2257,10 +2257,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="C156" s="0">
-        <v>0</v>
+        <v>1.5399123650249431</v>
       </c>
       <c r="D156" s="0">
-        <v>0</v>
+        <v>0.37370986206075041</v>
       </c>
     </row>
     <row r="157">
@@ -2271,10 +2271,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="C157" s="0">
-        <v>0</v>
+        <v>1.4966716660543578</v>
       </c>
       <c r="D157" s="0">
-        <v>0</v>
+        <v>0.36321609889946421</v>
       </c>
     </row>
     <row r="158">
@@ -2285,10 +2285,10 @@
         <v>4.2000000000000002</v>
       </c>
       <c r="C158" s="0">
-        <v>0</v>
+        <v>1.5617110066267903</v>
       </c>
       <c r="D158" s="0">
-        <v>0</v>
+        <v>0.35256802490180755</v>
       </c>
     </row>
     <row r="159">
@@ -2299,10 +2299,10 @@
         <v>4.2000000000000002</v>
       </c>
       <c r="C159" s="0">
-        <v>-2.0559501746274251</v>
+        <v>2.009315401921091</v>
       </c>
       <c r="D159" s="0">
-        <v>-0.46414624043060321</v>
+        <v>0.45361808916891067</v>
       </c>
     </row>
     <row r="160">
@@ -2313,10 +2313,10 @@
         <v>4.2000000000000002</v>
       </c>
       <c r="C160" s="0">
-        <v>0</v>
+        <v>1.9818072623352148</v>
       </c>
       <c r="D160" s="0">
-        <v>0</v>
+        <v>0.44740791942472491</v>
       </c>
     </row>
     <row r="161">
@@ -2327,10 +2327,10 @@
         <v>4.2000000000000002</v>
       </c>
       <c r="C161" s="0">
-        <v>0</v>
+        <v>1.9423998576927672</v>
       </c>
       <c r="D161" s="0">
-        <v>0</v>
+        <v>0.43851140095085955</v>
       </c>
     </row>
     <row r="162">
@@ -2341,10 +2341,10 @@
         <v>4.2000000000000002</v>
       </c>
       <c r="C162" s="0">
-        <v>0</v>
+        <v>1.8988473363558676</v>
       </c>
       <c r="D162" s="0">
-        <v>0</v>
+        <v>0.42867909115596931</v>
       </c>
     </row>
     <row r="163">
@@ -2355,10 +2355,10 @@
         <v>4.2000000000000002</v>
       </c>
       <c r="C163" s="0">
-        <v>0</v>
+        <v>1.8546767332597409</v>
       </c>
       <c r="D163" s="0">
-        <v>0</v>
+        <v>0.41870724474761223</v>
       </c>
     </row>
     <row r="164">
@@ -2369,10 +2369,10 @@
         <v>4.2000000000000002</v>
       </c>
       <c r="C164" s="0">
-        <v>0</v>
+        <v>1.8109225781158969</v>
       </c>
       <c r="D164" s="0">
-        <v>0</v>
+        <v>0.40882941460179523</v>
       </c>
     </row>
     <row r="165">
@@ -2383,10 +2383,10 @@
         <v>4.2000000000000002</v>
       </c>
       <c r="C165" s="0">
-        <v>0</v>
+        <v>1.7661316003013481</v>
       </c>
       <c r="D165" s="0">
-        <v>0</v>
+        <v>0.3987175139271591</v>
       </c>
     </row>
     <row r="166">
@@ -2397,10 +2397,10 @@
         <v>4.2000000000000002</v>
       </c>
       <c r="C166" s="0">
-        <v>0</v>
+        <v>1.7897760565943115</v>
       </c>
       <c r="D166" s="0">
-        <v>0</v>
+        <v>0.404055428060897</v>
       </c>
     </row>
     <row r="167">
@@ -2411,10 +2411,10 @@
         <v>4.2000000000000002</v>
       </c>
       <c r="C167" s="0">
-        <v>0</v>
+        <v>1.7453498635978442</v>
       </c>
       <c r="D167" s="0">
-        <v>0</v>
+        <v>0.39402588030705055</v>
       </c>
     </row>
     <row r="168">
@@ -2425,10 +2425,10 @@
         <v>4.2000000000000002</v>
       </c>
       <c r="C168" s="0">
-        <v>0</v>
+        <v>1.7006631292157723</v>
       </c>
       <c r="D168" s="0">
-        <v>0</v>
+        <v>0.38393751337261439</v>
       </c>
     </row>
     <row r="169">
@@ -2439,10 +2439,10 @@
         <v>4.2000000000000002</v>
       </c>
       <c r="C169" s="0">
-        <v>0</v>
+        <v>1.6553594303618353</v>
       </c>
       <c r="D169" s="0">
-        <v>0</v>
+        <v>0.37370986206075041</v>
       </c>
     </row>
     <row r="170">
@@ -2453,10 +2453,1466 @@
         <v>4.2000000000000002</v>
       </c>
       <c r="C170" s="0">
-        <v>0</v>
+        <v>1.6088769808133268</v>
       </c>
       <c r="D170" s="0">
-        <v>0</v>
+        <v>0.3632160988994641</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="0">
+        <v>10</v>
+      </c>
+      <c r="B171" s="0">
+        <v>4.2999999999999998</v>
+      </c>
+      <c r="C171" s="0">
+        <v>1.6759388430498352</v>
+      </c>
+      <c r="D171" s="0">
+        <v>0.35256802490180755</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="0">
+        <v>4</v>
+      </c>
+      <c r="B172" s="0">
+        <v>4.2999999999999998</v>
+      </c>
+      <c r="C172" s="0">
+        <v>2.1562822543534734</v>
+      </c>
+      <c r="D172" s="0">
+        <v>0.45361808916891067</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="B173" s="0">
+        <v>4.2999999999999998</v>
+      </c>
+      <c r="C173" s="0">
+        <v>2.1267620938139222</v>
+      </c>
+      <c r="D173" s="0">
+        <v>0.44740791942472491</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="0">
+        <v>5</v>
+      </c>
+      <c r="B174" s="0">
+        <v>4.2999999999999998</v>
+      </c>
+      <c r="C174" s="0">
+        <v>2.0844723232585411</v>
+      </c>
+      <c r="D174" s="0">
+        <v>0.43851140095085955</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="0">
+        <v>5.5</v>
+      </c>
+      <c r="B175" s="0">
+        <v>4.2999999999999998</v>
+      </c>
+      <c r="C175" s="0">
+        <v>2.0377342507780734</v>
+      </c>
+      <c r="D175" s="0">
+        <v>0.42867909115596925</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="0">
+        <v>6</v>
+      </c>
+      <c r="B176" s="0">
+        <v>4.2999999999999998</v>
+      </c>
+      <c r="C176" s="0">
+        <v>1.9903328883393014</v>
+      </c>
+      <c r="D176" s="0">
+        <v>0.41870724474761223</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="0">
+        <v>6.5</v>
+      </c>
+      <c r="B177" s="0">
+        <v>4.2999999999999998</v>
+      </c>
+      <c r="C177" s="0">
+        <v>1.9433784340009257</v>
+      </c>
+      <c r="D177" s="0">
+        <v>0.40882941460179528</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="0">
+        <v>7</v>
+      </c>
+      <c r="B178" s="0">
+        <v>4.2999999999999998</v>
+      </c>
+      <c r="C178" s="0">
+        <v>1.8953113209313144</v>
+      </c>
+      <c r="D178" s="0">
+        <v>0.39871751392715904</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="0">
+        <v>7.5</v>
+      </c>
+      <c r="B179" s="0">
+        <v>4.2999999999999998</v>
+      </c>
+      <c r="C179" s="0">
+        <v>1.9206851977600137</v>
+      </c>
+      <c r="D179" s="0">
+        <v>0.404055428060897</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="0">
+        <v>8</v>
+      </c>
+      <c r="B180" s="0">
+        <v>4.2999999999999998</v>
+      </c>
+      <c r="C180" s="0">
+        <v>1.8730095508729316</v>
+      </c>
+      <c r="D180" s="0">
+        <v>0.39402588030705055</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="0">
+        <v>8.5</v>
+      </c>
+      <c r="B181" s="0">
+        <v>4.2999999999999998</v>
+      </c>
+      <c r="C181" s="0">
+        <v>1.8250543058870312</v>
+      </c>
+      <c r="D181" s="0">
+        <v>0.38393751337261434</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="0">
+        <v>9</v>
+      </c>
+      <c r="B182" s="0">
+        <v>4.2999999999999998</v>
+      </c>
+      <c r="C182" s="0">
+        <v>1.7764369699516571</v>
+      </c>
+      <c r="D182" s="0">
+        <v>0.37370986206075035</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="0">
+        <v>9.5</v>
+      </c>
+      <c r="B183" s="0">
+        <v>4.2999999999999998</v>
+      </c>
+      <c r="C183" s="0">
+        <v>1.7265546662553335</v>
+      </c>
+      <c r="D183" s="0">
+        <v>0.36321609889946416</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="0">
+        <v>10</v>
+      </c>
+      <c r="B184" s="0">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C184" s="0">
+        <v>1.7956050964865626</v>
+      </c>
+      <c r="D184" s="0">
+        <v>0.35256802490180739</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="0">
+        <v>4</v>
+      </c>
+      <c r="B185" s="0">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C185" s="0">
+        <v>2.3102462368702921</v>
+      </c>
+      <c r="D185" s="0">
+        <v>0.45361808916891061</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="B186" s="0">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C186" s="0">
+        <v>2.2786182625359421</v>
+      </c>
+      <c r="D186" s="0">
+        <v>0.44740791942472474</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="0">
+        <v>5</v>
+      </c>
+      <c r="B187" s="0">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C187" s="0">
+        <v>2.2333088958765335</v>
+      </c>
+      <c r="D187" s="0">
+        <v>0.43851140095085939</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="0">
+        <v>5.5</v>
+      </c>
+      <c r="B188" s="0">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C188" s="0">
+        <v>2.183233607333686</v>
+      </c>
+      <c r="D188" s="0">
+        <v>0.42867909115596903</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="0">
+        <v>6</v>
+      </c>
+      <c r="B189" s="0">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C189" s="0">
+        <v>2.1324476682593358</v>
+      </c>
+      <c r="D189" s="0">
+        <v>0.41870724474761201</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="0">
+        <v>6.5</v>
+      </c>
+      <c r="B190" s="0">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C190" s="0">
+        <v>2.0821405476490726</v>
+      </c>
+      <c r="D190" s="0">
+        <v>0.40882941460179506</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="0">
+        <v>7</v>
+      </c>
+      <c r="B191" s="0">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C191" s="0">
+        <v>2.0306413216724706</v>
+      </c>
+      <c r="D191" s="0">
+        <v>0.39871751392715898</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="0">
+        <v>7.5</v>
+      </c>
+      <c r="B192" s="0">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C192" s="0">
+        <v>2.0578269571985981</v>
+      </c>
+      <c r="D192" s="0">
+        <v>0.40405542806089673</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="0">
+        <v>8</v>
+      </c>
+      <c r="B193" s="0">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C193" s="0">
+        <v>2.0067471490756761</v>
+      </c>
+      <c r="D193" s="0">
+        <v>0.39402588030705038</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="0">
+        <v>8.5</v>
+      </c>
+      <c r="B194" s="0">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C194" s="0">
+        <v>1.9553677788456472</v>
+      </c>
+      <c r="D194" s="0">
+        <v>0.38393751337261423</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="0">
+        <v>9</v>
+      </c>
+      <c r="B195" s="0">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C195" s="0">
+        <v>1.9032790427051951</v>
+      </c>
+      <c r="D195" s="0">
+        <v>0.37370986206075019</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="0">
+        <v>9.5</v>
+      </c>
+      <c r="B196" s="0">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C196" s="0">
+        <v>1.8498350169204512</v>
+      </c>
+      <c r="D196" s="0">
+        <v>0.36321609889946399</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="0">
+        <v>10</v>
+      </c>
+      <c r="B197" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="C197" s="0">
+        <v>1.9208362417512452</v>
+      </c>
+      <c r="D197" s="0">
+        <v>0.35256802490180755</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="0">
+        <v>4</v>
+      </c>
+      <c r="B198" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="C198" s="0">
+        <v>2.4713700734269977</v>
+      </c>
+      <c r="D198" s="0">
+        <v>0.45361808916891072</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="B199" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="C199" s="0">
+        <v>2.4375362647162349</v>
+      </c>
+      <c r="D199" s="0">
+        <v>0.44740791942472485</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="0">
+        <v>5</v>
+      </c>
+      <c r="B200" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="C200" s="0">
+        <v>2.3890668803619124</v>
+      </c>
+      <c r="D200" s="0">
+        <v>0.43851140095085955</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="0">
+        <v>5.5</v>
+      </c>
+      <c r="B201" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="C201" s="0">
+        <v>2.3354991837467387</v>
+      </c>
+      <c r="D201" s="0">
+        <v>0.42867909115596925</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="0">
+        <v>6</v>
+      </c>
+      <c r="B202" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="C202" s="0">
+        <v>2.2811712735975305</v>
+      </c>
+      <c r="D202" s="0">
+        <v>0.41870724474761217</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="0">
+        <v>6.5</v>
+      </c>
+      <c r="B203" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="C203" s="0">
+        <v>2.2273555762176205</v>
+      </c>
+      <c r="D203" s="0">
+        <v>0.40882941460179523</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="0">
+        <v>7</v>
+      </c>
+      <c r="B204" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="C204" s="0">
+        <v>2.1722646322948429</v>
+      </c>
+      <c r="D204" s="0">
+        <v>0.3987175139271591</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="0">
+        <v>7.5</v>
+      </c>
+      <c r="B205" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="C205" s="0">
+        <v>2.2013462795210641</v>
+      </c>
+      <c r="D205" s="0">
+        <v>0.40405542806089695</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="0">
+        <v>8</v>
+      </c>
+      <c r="B206" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="C206" s="0">
+        <v>2.1467040049718382</v>
+      </c>
+      <c r="D206" s="0">
+        <v>0.3940258803070506</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="0">
+        <v>8.5</v>
+      </c>
+      <c r="B207" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="C207" s="0">
+        <v>2.091741275912256</v>
+      </c>
+      <c r="D207" s="0">
+        <v>0.38393751337261434</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="0">
+        <v>9</v>
+      </c>
+      <c r="B208" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="C208" s="0">
+        <v>2.0360197075332329</v>
+      </c>
+      <c r="D208" s="0">
+        <v>0.3737098620607503</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="0">
+        <v>9.5</v>
+      </c>
+      <c r="B209" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="C209" s="0">
+        <v>1.9788483273487525</v>
+      </c>
+      <c r="D209" s="0">
+        <v>0.3632160988994641</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="0">
+        <v>10</v>
+      </c>
+      <c r="B210" s="0">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C210" s="0">
+        <v>2.0517587536581541</v>
+      </c>
+      <c r="D210" s="0">
+        <v>0.35256802490180783</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="0">
+        <v>4</v>
+      </c>
+      <c r="B211" s="0">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C211" s="0">
+        <v>2.6398164879790431</v>
+      </c>
+      <c r="D211" s="0">
+        <v>0.45361808916891094</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="B212" s="0">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C212" s="0">
+        <v>2.6036765965697612</v>
+      </c>
+      <c r="D212" s="0">
+        <v>0.44740791942472508</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="0">
+        <v>5</v>
+      </c>
+      <c r="B213" s="0">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C213" s="0">
+        <v>2.5519035815298454</v>
+      </c>
+      <c r="D213" s="0">
+        <v>0.43851140095085972</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="0">
+        <v>5.5</v>
+      </c>
+      <c r="B214" s="0">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C214" s="0">
+        <v>2.4946847577412639</v>
+      </c>
+      <c r="D214" s="0">
+        <v>0.42867909115596953</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="0">
+        <v>6</v>
+      </c>
+      <c r="B215" s="0">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C215" s="0">
+        <v>2.4366539049315694</v>
+      </c>
+      <c r="D215" s="0">
+        <v>0.41870724474761234</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="0">
+        <v>6.5</v>
+      </c>
+      <c r="B216" s="0">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C216" s="0">
+        <v>2.3791701768638505</v>
+      </c>
+      <c r="D216" s="0">
+        <v>0.40882941460179539</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="0">
+        <v>7</v>
+      </c>
+      <c r="B217" s="0">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C217" s="0">
+        <v>2.3203242825684596</v>
+      </c>
+      <c r="D217" s="0">
+        <v>0.39871751392715926</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="0">
+        <v>7.5</v>
+      </c>
+      <c r="B218" s="0">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C218" s="0">
+        <v>2.3513881093384077</v>
+      </c>
+      <c r="D218" s="0">
+        <v>0.40405542806089728</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="0">
+        <v>8</v>
+      </c>
+      <c r="B219" s="0">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C219" s="0">
+        <v>2.2930214653271759</v>
+      </c>
+      <c r="D219" s="0">
+        <v>0.39402588030705082</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="0">
+        <v>8.5</v>
+      </c>
+      <c r="B220" s="0">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C220" s="0">
+        <v>2.2343125249074944</v>
+      </c>
+      <c r="D220" s="0">
+        <v>0.38393751337261461</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="0">
+        <v>9</v>
+      </c>
+      <c r="B221" s="0">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C221" s="0">
+        <v>2.1747930233465556</v>
+      </c>
+      <c r="D221" s="0">
+        <v>0.37370986206075058</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="0">
+        <v>9.5</v>
+      </c>
+      <c r="B222" s="0">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C222" s="0">
+        <v>2.11372489208031</v>
+      </c>
+      <c r="D222" s="0">
+        <v>0.36321609889946432</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="0">
+        <v>10</v>
+      </c>
+      <c r="B223" s="0">
+        <v>4.7000000000000002</v>
+      </c>
+      <c r="C223" s="0">
+        <v>2.1884991070215594</v>
+      </c>
+      <c r="D223" s="0">
+        <v>0.35256802490180766</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="0">
+        <v>4</v>
+      </c>
+      <c r="B224" s="0">
+        <v>4.7000000000000002</v>
+      </c>
+      <c r="C224" s="0">
+        <v>2.8157482044818796</v>
+      </c>
+      <c r="D224" s="0">
+        <v>0.45361808916891089</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="B225" s="0">
+        <v>4.7000000000000002</v>
+      </c>
+      <c r="C225" s="0">
+        <v>2.7771997543114808</v>
+      </c>
+      <c r="D225" s="0">
+        <v>0.44740791942472491</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="0">
+        <v>5</v>
+      </c>
+      <c r="B226" s="0">
+        <v>4.7000000000000002</v>
+      </c>
+      <c r="C226" s="0">
+        <v>2.7219763041954996</v>
+      </c>
+      <c r="D226" s="0">
+        <v>0.43851140095085966</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="0">
+        <v>5.5</v>
+      </c>
+      <c r="B227" s="0">
+        <v>4.7000000000000002</v>
+      </c>
+      <c r="C227" s="0">
+        <v>2.6609441070412925</v>
+      </c>
+      <c r="D227" s="0">
+        <v>0.42867909115596942</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="0">
+        <v>6</v>
+      </c>
+      <c r="B228" s="0">
+        <v>4.7000000000000002</v>
+      </c>
+      <c r="C228" s="0">
+        <v>2.5990457628391379</v>
+      </c>
+      <c r="D228" s="0">
+        <v>0.41870724474761223</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="0">
+        <v>6.5</v>
+      </c>
+      <c r="B229" s="0">
+        <v>4.7000000000000002</v>
+      </c>
+      <c r="C229" s="0">
+        <v>2.5377310067450427</v>
+      </c>
+      <c r="D229" s="0">
+        <v>0.40882941460179517</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="0">
+        <v>7</v>
+      </c>
+      <c r="B230" s="0">
+        <v>4.7000000000000002</v>
+      </c>
+      <c r="C230" s="0">
+        <v>2.474963302263347</v>
+      </c>
+      <c r="D230" s="0">
+        <v>0.3987175139271591</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="0">
+        <v>7.5</v>
+      </c>
+      <c r="B231" s="0">
+        <v>4.7000000000000002</v>
+      </c>
+      <c r="C231" s="0">
+        <v>2.5080973912616242</v>
+      </c>
+      <c r="D231" s="0">
+        <v>0.40405542806089706</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="0">
+        <v>8</v>
+      </c>
+      <c r="B232" s="0">
+        <v>4.7000000000000002</v>
+      </c>
+      <c r="C232" s="0">
+        <v>2.445840876907448</v>
+      </c>
+      <c r="D232" s="0">
+        <v>0.39402588030705066</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="0">
+        <v>8.5</v>
+      </c>
+      <c r="B233" s="0">
+        <v>4.7000000000000002</v>
+      </c>
+      <c r="C233" s="0">
+        <v>2.3832192536519967</v>
+      </c>
+      <c r="D233" s="0">
+        <v>0.38393751337261439</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="0">
+        <v>9</v>
+      </c>
+      <c r="B234" s="0">
+        <v>4.7000000000000002</v>
+      </c>
+      <c r="C234" s="0">
+        <v>2.3197330490559445</v>
+      </c>
+      <c r="D234" s="0">
+        <v>0.37370986206075041</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="0">
+        <v>9.5</v>
+      </c>
+      <c r="B235" s="0">
+        <v>4.7000000000000002</v>
+      </c>
+      <c r="C235" s="0">
+        <v>2.2545950056551938</v>
+      </c>
+      <c r="D235" s="0">
+        <v>0.3632160988994641</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="0">
+        <v>10</v>
+      </c>
+      <c r="B236" s="0">
+        <v>4.7999999999999998</v>
+      </c>
+      <c r="C236" s="0">
+        <v>2.3311837766557346</v>
+      </c>
+      <c r="D236" s="0">
+        <v>0.35256802490180777</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="0">
+        <v>4</v>
+      </c>
+      <c r="B237" s="0">
+        <v>4.7999999999999998</v>
+      </c>
+      <c r="C237" s="0">
+        <v>2.9993279468909586</v>
+      </c>
+      <c r="D237" s="0">
+        <v>0.45361808916891089</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="B238" s="0">
+        <v>4.7999999999999998</v>
+      </c>
+      <c r="C238" s="0">
+        <v>2.9582662341563566</v>
+      </c>
+      <c r="D238" s="0">
+        <v>0.44740791942472519</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="0">
+        <v>5</v>
+      </c>
+      <c r="B239" s="0">
+        <v>4.7999999999999998</v>
+      </c>
+      <c r="C239" s="0">
+        <v>2.8994423531740434</v>
+      </c>
+      <c r="D239" s="0">
+        <v>0.43851140095085972</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="0">
+        <v>5.5</v>
+      </c>
+      <c r="B240" s="0">
+        <v>4.7999999999999998</v>
+      </c>
+      <c r="C240" s="0">
+        <v>2.8344310093708582</v>
+      </c>
+      <c r="D240" s="0">
+        <v>0.42867909115596953</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" s="0">
+        <v>6</v>
+      </c>
+      <c r="B241" s="0">
+        <v>4.7999999999999998</v>
+      </c>
+      <c r="C241" s="0">
+        <v>2.7684970478979229</v>
+      </c>
+      <c r="D241" s="0">
+        <v>0.41870724474761245</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="0">
+        <v>6.5</v>
+      </c>
+      <c r="B242" s="0">
+        <v>4.7999999999999998</v>
+      </c>
+      <c r="C242" s="0">
+        <v>2.7031847230184822</v>
+      </c>
+      <c r="D242" s="0">
+        <v>0.40882941460179545</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="0">
+        <v>7</v>
+      </c>
+      <c r="B243" s="0">
+        <v>4.7999999999999998</v>
+      </c>
+      <c r="C243" s="0">
+        <v>2.6363247211495349</v>
+      </c>
+      <c r="D243" s="0">
+        <v>0.39871751392715932</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="0">
+        <v>7.5</v>
+      </c>
+      <c r="B244" s="0">
+        <v>4.7999999999999998</v>
+      </c>
+      <c r="C244" s="0">
+        <v>2.6716190699017131</v>
+      </c>
+      <c r="D244" s="0">
+        <v>0.40405542806089717</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="0">
+        <v>8</v>
+      </c>
+      <c r="B245" s="0">
+        <v>4.7999999999999998</v>
+      </c>
+      <c r="C245" s="0">
+        <v>2.6053035864784158</v>
+      </c>
+      <c r="D245" s="0">
+        <v>0.39402588030705082</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="0">
+        <v>8.5</v>
+      </c>
+      <c r="B246" s="0">
+        <v>4.7999999999999998</v>
+      </c>
+      <c r="C246" s="0">
+        <v>2.5385991899664013</v>
+      </c>
+      <c r="D246" s="0">
+        <v>0.38393751337261456</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="0">
+        <v>9</v>
+      </c>
+      <c r="B247" s="0">
+        <v>4.7999999999999998</v>
+      </c>
+      <c r="C247" s="0">
+        <v>2.4709738435721857</v>
+      </c>
+      <c r="D247" s="0">
+        <v>0.37370986206075052</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" s="0">
+        <v>9.5</v>
+      </c>
+      <c r="B248" s="0">
+        <v>4.7999999999999998</v>
+      </c>
+      <c r="C248" s="0">
+        <v>2.4015889626134799</v>
+      </c>
+      <c r="D248" s="0">
+        <v>0.36321609889946432</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="0">
+        <v>10</v>
+      </c>
+      <c r="B249" s="0">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C249" s="0">
+        <v>2.4799392373749503</v>
+      </c>
+      <c r="D249" s="0">
+        <v>0.35256802490180761</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="0">
+        <v>4</v>
+      </c>
+      <c r="B250" s="0">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C250" s="0">
+        <v>3.1907184391617331</v>
+      </c>
+      <c r="D250" s="0">
+        <v>0.45361808916891072</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="B251" s="0">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C251" s="0">
+        <v>3.1470365323193463</v>
+      </c>
+      <c r="D251" s="0">
+        <v>0.44740791942472496</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="0">
+        <v>5</v>
+      </c>
+      <c r="B252" s="0">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C252" s="0">
+        <v>3.0844590332806447</v>
+      </c>
+      <c r="D252" s="0">
+        <v>0.43851140095085961</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="0">
+        <v>5.5</v>
+      </c>
+      <c r="B253" s="0">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C253" s="0">
+        <v>3.0152992424539935</v>
+      </c>
+      <c r="D253" s="0">
+        <v>0.42867909115596925</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="0">
+        <v>6</v>
+      </c>
+      <c r="B254" s="0">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C254" s="0">
+        <v>2.9451579606856071</v>
+      </c>
+      <c r="D254" s="0">
+        <v>0.41870724474761217</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="0">
+        <v>6.5</v>
+      </c>
+      <c r="B255" s="0">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C255" s="0">
+        <v>2.8756779828414474</v>
+      </c>
+      <c r="D255" s="0">
+        <v>0.40882941460179517</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="0">
+        <v>7</v>
+      </c>
+      <c r="B256" s="0">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C256" s="0">
+        <v>2.8045515689970486</v>
+      </c>
+      <c r="D256" s="0">
+        <v>0.3987175139271591</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" s="0">
+        <v>7.5</v>
+      </c>
+      <c r="B257" s="0">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C257" s="0">
+        <v>2.8420980898696708</v>
+      </c>
+      <c r="D257" s="0">
+        <v>0.404055428060897</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="0">
+        <v>8</v>
+      </c>
+      <c r="B258" s="0">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C258" s="0">
+        <v>2.7715509408058359</v>
+      </c>
+      <c r="D258" s="0">
+        <v>0.39402588030705049</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="0">
+        <v>8.5</v>
+      </c>
+      <c r="B259" s="0">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C259" s="0">
+        <v>2.7005900616713427</v>
+      </c>
+      <c r="D259" s="0">
+        <v>0.38393751337261439</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" s="0">
+        <v>9</v>
+      </c>
+      <c r="B260" s="0">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C260" s="0">
+        <v>2.6286494658060624</v>
+      </c>
+      <c r="D260" s="0">
+        <v>0.37370986206075035</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="0">
+        <v>9.5</v>
+      </c>
+      <c r="B261" s="0">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C261" s="0">
+        <v>2.5548370574952366</v>
+      </c>
+      <c r="D261" s="0">
+        <v>0.3632160988994641</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="0">
+        <v>10</v>
+      </c>
+      <c r="B262" s="0">
+        <v>5</v>
+      </c>
+      <c r="C262" s="0">
+        <v>2.6348919639934776</v>
+      </c>
+      <c r="D262" s="0">
+        <v>0.35256802490180755</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" s="0">
+        <v>4</v>
+      </c>
+      <c r="B263" s="0">
+        <v>5</v>
+      </c>
+      <c r="C263" s="0">
+        <v>3.3900824052496543</v>
+      </c>
+      <c r="D263" s="0">
+        <v>0.45361808916891078</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="B264" s="0">
+        <v>5</v>
+      </c>
+      <c r="C264" s="0">
+        <v>3.3436711450154113</v>
+      </c>
+      <c r="D264" s="0">
+        <v>0.44740791942472491</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" s="0">
+        <v>5</v>
+      </c>
+      <c r="B265" s="0">
+        <v>5</v>
+      </c>
+      <c r="C265" s="0">
+        <v>3.2771836493304702</v>
+      </c>
+      <c r="D265" s="0">
+        <v>0.43851140095085961</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" s="0">
+        <v>5.5</v>
+      </c>
+      <c r="B266" s="0">
+        <v>5</v>
+      </c>
+      <c r="C266" s="0">
+        <v>3.2037025840147311</v>
+      </c>
+      <c r="D266" s="0">
+        <v>0.42867909115596931</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" s="0">
+        <v>6</v>
+      </c>
+      <c r="B267" s="0">
+        <v>5</v>
+      </c>
+      <c r="C267" s="0">
+        <v>3.1291787017798773</v>
+      </c>
+      <c r="D267" s="0">
+        <v>0.41870724474761223</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="0">
+        <v>6.5</v>
+      </c>
+      <c r="B268" s="0">
+        <v>5</v>
+      </c>
+      <c r="C268" s="0">
+        <v>3.0553574433712214</v>
+      </c>
+      <c r="D268" s="0">
+        <v>0.40882941460179523</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" s="0">
+        <v>7</v>
+      </c>
+      <c r="B269" s="0">
+        <v>5</v>
+      </c>
+      <c r="C269" s="0">
+        <v>2.979786875575916</v>
+      </c>
+      <c r="D269" s="0">
+        <v>0.3987175139271591</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" s="0">
+        <v>7.5</v>
+      </c>
+      <c r="B270" s="0">
+        <v>5</v>
+      </c>
+      <c r="C270" s="0">
+        <v>3.0196793957764942</v>
+      </c>
+      <c r="D270" s="0">
+        <v>0.404055428060897</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" s="0">
+        <v>8</v>
+      </c>
+      <c r="B271" s="0">
+        <v>5</v>
+      </c>
+      <c r="C271" s="0">
+        <v>2.9447242866554704</v>
+      </c>
+      <c r="D271" s="0">
+        <v>0.39402588030705055</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="0">
+        <v>8.5</v>
+      </c>
+      <c r="B272" s="0">
+        <v>5</v>
+      </c>
+      <c r="C272" s="0">
+        <v>2.8693295965874568</v>
+      </c>
+      <c r="D272" s="0">
+        <v>0.38393751337261439</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" s="0">
+        <v>9</v>
+      </c>
+      <c r="B273" s="0">
+        <v>5</v>
+      </c>
+      <c r="C273" s="0">
+        <v>2.7928939746683583</v>
+      </c>
+      <c r="D273" s="0">
+        <v>0.37370986206075035</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" s="0">
+        <v>9.5</v>
+      </c>
+      <c r="B274" s="0">
+        <v>5</v>
+      </c>
+      <c r="C274" s="0">
+        <v>2.7144695848405385</v>
+      </c>
+      <c r="D274" s="0">
+        <v>0.3632160988994641</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes velocity range to 3 to 7; delete test results
</commit_message>
<xml_diff>
--- a/Data/output_results.xlsx
+++ b/Data/output_results.xlsx
@@ -13,7 +13,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>u1</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Cp</t>
+  </si>
   <si>
     <t>alpha</t>
   </si>
@@ -81,16 +93,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2">
@@ -280,10 +292,10 @@
         <v>10</v>
       </c>
       <c r="B15" s="0">
-        <v>3.1000000000000001</v>
+        <v>3.2000000000000002</v>
       </c>
       <c r="C15" s="0">
-        <v>0.62796853199463776</v>
+        <v>0.69072111900910649</v>
       </c>
       <c r="D15" s="0">
         <v>0.35256802490180766</v>
@@ -294,10 +306,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="0">
-        <v>3.1000000000000001</v>
+        <v>3.2000000000000002</v>
       </c>
       <c r="C16" s="0">
-        <v>0.80795155947833952</v>
+        <v>0.88868976204176531</v>
       </c>
       <c r="D16" s="0">
         <v>0.45361808916891067</v>
@@ -308,10 +320,10 @@
         <v>4.5</v>
       </c>
       <c r="B17" s="0">
-        <v>3.1000000000000001</v>
+        <v>3.2000000000000002</v>
       </c>
       <c r="C17" s="0">
-        <v>0.79689045664923308</v>
+        <v>0.87652332863892024</v>
       </c>
       <c r="D17" s="0">
         <v>0.44740791942472491</v>
@@ -322,13 +334,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="0">
-        <v>3.1000000000000001</v>
+        <v>3.2000000000000002</v>
       </c>
       <c r="C18" s="0">
-        <v>0.78104462477763237</v>
+        <v>0.85909403057008704</v>
       </c>
       <c r="D18" s="0">
-        <v>0.43851140095085961</v>
+        <v>0.43851140095085966</v>
       </c>
     </row>
     <row r="19">
@@ -336,13 +348,13 @@
         <v>5.5</v>
       </c>
       <c r="B19" s="0">
-        <v>3.1000000000000001</v>
+        <v>3.2000000000000002</v>
       </c>
       <c r="C19" s="0">
-        <v>0.76353202944306309</v>
+        <v>0.8398314101839579</v>
       </c>
       <c r="D19" s="0">
-        <v>0.42867909115596936</v>
+        <v>0.42867909115596931</v>
       </c>
     </row>
     <row r="20">
@@ -350,13 +362,13 @@
         <v>6</v>
       </c>
       <c r="B20" s="0">
-        <v>3.1000000000000001</v>
+        <v>3.2000000000000002</v>
       </c>
       <c r="C20" s="0">
-        <v>0.74577090163779469</v>
+        <v>0.82029542159938407</v>
       </c>
       <c r="D20" s="0">
-        <v>0.41870724474761223</v>
+        <v>0.41870724474761206</v>
       </c>
     </row>
     <row r="21">
@@ -364,13 +376,13 @@
         <v>6.5</v>
       </c>
       <c r="B21" s="0">
-        <v>3.1000000000000001</v>
+        <v>3.2000000000000002</v>
       </c>
       <c r="C21" s="0">
-        <v>0.72817722876377655</v>
+        <v>0.80094362163510546</v>
       </c>
       <c r="D21" s="0">
-        <v>0.40882941460179517</v>
+        <v>0.40882941460179512</v>
       </c>
     </row>
     <row r="22">
@@ -378,13 +390,13 @@
         <v>7</v>
       </c>
       <c r="B22" s="0">
-        <v>3.1000000000000001</v>
+        <v>3.2000000000000002</v>
       </c>
       <c r="C22" s="0">
-        <v>0.71016664648225702</v>
+        <v>0.78113325071097306</v>
       </c>
       <c r="D22" s="0">
-        <v>0.3987175139271591</v>
+        <v>0.39871751392715904</v>
       </c>
     </row>
     <row r="23">
@@ -392,13 +404,13 @@
         <v>7.5</v>
       </c>
       <c r="B23" s="0">
-        <v>3.1000000000000001</v>
+        <v>3.2000000000000002</v>
       </c>
       <c r="C23" s="0">
-        <v>0.71967415103662047</v>
+        <v>0.79159083552643328</v>
       </c>
       <c r="D23" s="0">
-        <v>0.40405542806089706</v>
+        <v>0.40405542806089689</v>
       </c>
     </row>
     <row r="24">
@@ -406,13 +418,13 @@
         <v>8</v>
       </c>
       <c r="B24" s="0">
-        <v>3.1000000000000001</v>
+        <v>3.2000000000000002</v>
       </c>
       <c r="C24" s="0">
-        <v>0.70181024979002493</v>
+        <v>0.77194180340101171</v>
       </c>
       <c r="D24" s="0">
-        <v>0.39402588030705049</v>
+        <v>0.39402588030705055</v>
       </c>
     </row>
     <row r="25">
@@ -420,13 +432,13 @@
         <v>8.5</v>
       </c>
       <c r="B25" s="0">
-        <v>3.1000000000000001</v>
+        <v>3.2000000000000002</v>
       </c>
       <c r="C25" s="0">
-        <v>0.68384158409549556</v>
+        <v>0.75217753776782237</v>
       </c>
       <c r="D25" s="0">
-        <v>0.38393751337261439</v>
+        <v>0.38393751337261434</v>
       </c>
     </row>
     <row r="26">
@@ -434,13 +446,13 @@
         <v>9</v>
       </c>
       <c r="B26" s="0">
-        <v>3.1000000000000001</v>
+        <v>3.2000000000000002</v>
       </c>
       <c r="C26" s="0">
-        <v>0.66562483519476057</v>
+        <v>0.73214039809546227</v>
       </c>
       <c r="D26" s="0">
-        <v>0.3737098620607503</v>
+        <v>0.37370986206075035</v>
       </c>
     </row>
     <row r="27">
@@ -448,10 +460,10 @@
         <v>9.5</v>
       </c>
       <c r="B27" s="0">
-        <v>3.1000000000000001</v>
+        <v>3.2000000000000002</v>
       </c>
       <c r="C27" s="0">
-        <v>0.64693410721587596</v>
+        <v>0.71158191484843836</v>
       </c>
       <c r="D27" s="0">
         <v>0.36321609889946416</v>
@@ -462,13 +474,13 @@
         <v>10</v>
       </c>
       <c r="B28" s="0">
-        <v>3.2000000000000002</v>
+        <v>3.3999999999999999</v>
       </c>
       <c r="C28" s="0">
-        <v>0.69072111900910649</v>
+        <v>0.82849435002239713</v>
       </c>
       <c r="D28" s="0">
-        <v>0.35256802490180766</v>
+        <v>0.35256802490180755</v>
       </c>
     </row>
     <row r="29">
@@ -476,13 +488,13 @@
         <v>4</v>
       </c>
       <c r="B29" s="0">
-        <v>3.2000000000000002</v>
+        <v>3.3999999999999999</v>
       </c>
       <c r="C29" s="0">
-        <v>0.88868976204176531</v>
+        <v>1.0659503908474592</v>
       </c>
       <c r="D29" s="0">
-        <v>0.45361808916891067</v>
+        <v>0.45361808916891078</v>
       </c>
     </row>
     <row r="30">
@@ -490,10 +502,10 @@
         <v>4.5</v>
       </c>
       <c r="B30" s="0">
-        <v>3.2000000000000002</v>
+        <v>3.3999999999999999</v>
       </c>
       <c r="C30" s="0">
-        <v>0.87652332863892024</v>
+        <v>1.0513572054694857</v>
       </c>
       <c r="D30" s="0">
         <v>0.44740791942472491</v>
@@ -504,10 +516,10 @@
         <v>5</v>
       </c>
       <c r="B31" s="0">
-        <v>3.2000000000000002</v>
+        <v>3.3999999999999999</v>
       </c>
       <c r="C31" s="0">
-        <v>0.85909403057008704</v>
+        <v>1.0304514092262784</v>
       </c>
       <c r="D31" s="0">
         <v>0.43851140095085966</v>
@@ -518,13 +530,13 @@
         <v>5.5</v>
       </c>
       <c r="B32" s="0">
-        <v>3.2000000000000002</v>
+        <v>3.3999999999999999</v>
       </c>
       <c r="C32" s="0">
-        <v>0.8398314101839579</v>
+        <v>1.0073466108969198</v>
       </c>
       <c r="D32" s="0">
-        <v>0.42867909115596931</v>
+        <v>0.42867909115596925</v>
       </c>
     </row>
     <row r="33">
@@ -532,13 +544,13 @@
         <v>6</v>
       </c>
       <c r="B33" s="0">
-        <v>3.2000000000000002</v>
+        <v>3.3999999999999999</v>
       </c>
       <c r="C33" s="0">
-        <v>0.82029542159938407</v>
+        <v>0.98391391755805047</v>
       </c>
       <c r="D33" s="0">
-        <v>0.41870724474761206</v>
+        <v>0.41870724474761228</v>
       </c>
     </row>
     <row r="34">
@@ -546,13 +558,13 @@
         <v>6.5</v>
       </c>
       <c r="B34" s="0">
-        <v>3.2000000000000002</v>
+        <v>3.3999999999999999</v>
       </c>
       <c r="C34" s="0">
-        <v>0.80094362163510546</v>
+        <v>0.9607021516341</v>
       </c>
       <c r="D34" s="0">
-        <v>0.40882941460179512</v>
+        <v>0.40882941460179528</v>
       </c>
     </row>
     <row r="35">
@@ -560,13 +572,13 @@
         <v>7</v>
       </c>
       <c r="B35" s="0">
-        <v>3.2000000000000002</v>
+        <v>3.3999999999999999</v>
       </c>
       <c r="C35" s="0">
-        <v>0.78113325071097306</v>
+        <v>0.93694034686108651</v>
       </c>
       <c r="D35" s="0">
-        <v>0.39871751392715904</v>
+        <v>0.39871751392715915</v>
       </c>
     </row>
     <row r="36">
@@ -574,13 +586,13 @@
         <v>7.5</v>
       </c>
       <c r="B36" s="0">
-        <v>3.2000000000000002</v>
+        <v>3.3999999999999999</v>
       </c>
       <c r="C36" s="0">
-        <v>0.79159083552643328</v>
+        <v>0.94948383177279472</v>
       </c>
       <c r="D36" s="0">
-        <v>0.40405542806089689</v>
+        <v>0.40405542806089706</v>
       </c>
     </row>
     <row r="37">
@@ -588,13 +600,13 @@
         <v>8</v>
       </c>
       <c r="B37" s="0">
-        <v>3.2000000000000002</v>
+        <v>3.3999999999999999</v>
       </c>
       <c r="C37" s="0">
-        <v>0.77194180340101171</v>
+        <v>0.92591554690165301</v>
       </c>
       <c r="D37" s="0">
-        <v>0.39402588030705055</v>
+        <v>0.39402588030705066</v>
       </c>
     </row>
     <row r="38">
@@ -602,13 +614,13 @@
         <v>8.5</v>
       </c>
       <c r="B38" s="0">
-        <v>3.2000000000000002</v>
+        <v>3.3999999999999999</v>
       </c>
       <c r="C38" s="0">
-        <v>0.75217753776782237</v>
+        <v>0.90220904371418731</v>
       </c>
       <c r="D38" s="0">
-        <v>0.38393751337261434</v>
+        <v>0.38393751337261439</v>
       </c>
     </row>
     <row r="39">
@@ -616,10 +628,10 @@
         <v>9</v>
       </c>
       <c r="B39" s="0">
-        <v>3.2000000000000002</v>
+        <v>3.3999999999999999</v>
       </c>
       <c r="C39" s="0">
-        <v>0.73214039809546227</v>
+        <v>0.87817523824292121</v>
       </c>
       <c r="D39" s="0">
         <v>0.37370986206075035</v>
@@ -630,13 +642,13 @@
         <v>9.5</v>
       </c>
       <c r="B40" s="0">
-        <v>3.2000000000000002</v>
+        <v>3.3999999999999999</v>
       </c>
       <c r="C40" s="0">
-        <v>0.71158191484843836</v>
+        <v>0.85351610050058035</v>
       </c>
       <c r="D40" s="0">
-        <v>0.36321609889946416</v>
+        <v>0.36321609889946421</v>
       </c>
     </row>
     <row r="41">
@@ -644,13 +656,13 @@
         <v>10</v>
       </c>
       <c r="B41" s="0">
-        <v>3.2999999999999998</v>
+        <v>3.6000000000000001</v>
       </c>
       <c r="C41" s="0">
-        <v>0.75752090008026896</v>
+        <v>0.9834681557766376</v>
       </c>
       <c r="D41" s="0">
-        <v>0.35256802490180761</v>
+        <v>0.3525680249018075</v>
       </c>
     </row>
     <row r="42">
@@ -658,13 +670,13 @@
         <v>4</v>
       </c>
       <c r="B42" s="0">
-        <v>3.2999999999999998</v>
+        <v>3.6000000000000001</v>
       </c>
       <c r="C42" s="0">
-        <v>0.97463513117965439</v>
+        <v>1.2653414775946232</v>
       </c>
       <c r="D42" s="0">
-        <v>0.45361808916891067</v>
+        <v>0.45361808916891078</v>
       </c>
     </row>
     <row r="43">
@@ -672,10 +684,10 @@
         <v>4.5</v>
       </c>
       <c r="B43" s="0">
-        <v>3.2999999999999998</v>
+        <v>3.6000000000000001</v>
       </c>
       <c r="C43" s="0">
-        <v>0.96129207950735063</v>
+        <v>1.2480185675347124</v>
       </c>
       <c r="D43" s="0">
         <v>0.44740791942472485</v>
@@ -686,13 +698,13 @@
         <v>5</v>
       </c>
       <c r="B44" s="0">
-        <v>3.2999999999999998</v>
+        <v>3.6000000000000001</v>
       </c>
       <c r="C44" s="0">
-        <v>0.94217719044791282</v>
+        <v>1.2232022427452993</v>
       </c>
       <c r="D44" s="0">
-        <v>0.43851140095085961</v>
+        <v>0.4385114009508595</v>
       </c>
     </row>
     <row r="45">
@@ -700,13 +712,13 @@
         <v>5.5</v>
       </c>
       <c r="B45" s="0">
-        <v>3.2999999999999998</v>
+        <v>3.6000000000000001</v>
       </c>
       <c r="C45" s="0">
-        <v>0.92105167809389932</v>
+        <v>1.1957755820783305</v>
       </c>
       <c r="D45" s="0">
-        <v>0.42867909115596936</v>
+        <v>0.42867909115596925</v>
       </c>
     </row>
     <row r="46">
@@ -714,10 +726,10 @@
         <v>6</v>
       </c>
       <c r="B46" s="0">
-        <v>3.2999999999999998</v>
+        <v>3.6000000000000001</v>
       </c>
       <c r="C46" s="0">
-        <v>0.89962636004690755</v>
+        <v>1.1679596920819357</v>
       </c>
       <c r="D46" s="0">
         <v>0.41870724474761217</v>
@@ -728,13 +740,13 @@
         <v>6.5</v>
       </c>
       <c r="B47" s="0">
-        <v>3.2999999999999998</v>
+        <v>3.6000000000000001</v>
       </c>
       <c r="C47" s="0">
-        <v>0.87840304353945275</v>
+        <v>1.1404060550234221</v>
       </c>
       <c r="D47" s="0">
-        <v>0.40882941460179523</v>
+        <v>0.40882941460179528</v>
       </c>
     </row>
     <row r="48">
@@ -742,10 +754,10 @@
         <v>7</v>
       </c>
       <c r="B48" s="0">
-        <v>3.2999999999999998</v>
+        <v>3.6000000000000001</v>
       </c>
       <c r="C48" s="0">
-        <v>0.85667680758057363</v>
+        <v>1.1121994917349598</v>
       </c>
       <c r="D48" s="0">
         <v>0.3987175139271591</v>
@@ -756,10 +768,10 @@
         <v>7.5</v>
       </c>
       <c r="B49" s="0">
-        <v>3.2999999999999998</v>
+        <v>3.6000000000000001</v>
       </c>
       <c r="C49" s="0">
-        <v>0.86814574756815899</v>
+        <v>1.1270892951147851</v>
       </c>
       <c r="D49" s="0">
         <v>0.404055428060897</v>
@@ -770,13 +782,13 @@
         <v>8</v>
       </c>
       <c r="B50" s="0">
-        <v>3.2999999999999998</v>
+        <v>3.6000000000000001</v>
       </c>
       <c r="C50" s="0">
-        <v>0.84659645351630131</v>
+        <v>1.0991124505455814</v>
       </c>
       <c r="D50" s="0">
-        <v>0.39402588030705066</v>
+        <v>0.3940258803070506</v>
       </c>
     </row>
     <row r="51">
@@ -784,13 +796,13 @@
         <v>8.5</v>
       </c>
       <c r="B51" s="0">
-        <v>3.2999999999999998</v>
+        <v>3.6000000000000001</v>
       </c>
       <c r="C51" s="0">
-        <v>0.82492078170050753</v>
+        <v>1.0709715332670755</v>
       </c>
       <c r="D51" s="0">
-        <v>0.38393751337261439</v>
+        <v>0.38393751337261445</v>
       </c>
     </row>
     <row r="52">
@@ -798,13 +810,13 @@
         <v>9</v>
       </c>
       <c r="B52" s="0">
-        <v>3.2999999999999998</v>
+        <v>3.6000000000000001</v>
       </c>
       <c r="C52" s="0">
-        <v>0.80294584614125442</v>
+        <v>1.0424420902570155</v>
       </c>
       <c r="D52" s="0">
-        <v>0.37370986206075035</v>
+        <v>0.3737098620607503</v>
       </c>
     </row>
     <row r="53">
@@ -812,13 +824,13 @@
         <v>9.5</v>
       </c>
       <c r="B53" s="0">
-        <v>3.2999999999999998</v>
+        <v>3.6000000000000001</v>
       </c>
       <c r="C53" s="0">
-        <v>0.78039914776331543</v>
+        <v>1.0131703436025616</v>
       </c>
       <c r="D53" s="0">
-        <v>0.3632160988994641</v>
+        <v>0.36321609889946416</v>
       </c>
     </row>
     <row r="54">
@@ -826,13 +838,13 @@
         <v>10</v>
       </c>
       <c r="B54" s="0">
-        <v>3.3999999999999999</v>
+        <v>3.7999999999999998</v>
       </c>
       <c r="C54" s="0">
-        <v>0.82849435002239713</v>
+        <v>1.156654334786001</v>
       </c>
       <c r="D54" s="0">
-        <v>0.35256802490180755</v>
+        <v>0.35256802490180766</v>
       </c>
     </row>
     <row r="55">
@@ -840,13 +852,13 @@
         <v>4</v>
       </c>
       <c r="B55" s="0">
-        <v>3.3999999999999999</v>
+        <v>3.7999999999999998</v>
       </c>
       <c r="C55" s="0">
-        <v>1.0659503908474592</v>
+        <v>1.4881648139268726</v>
       </c>
       <c r="D55" s="0">
-        <v>0.45361808916891078</v>
+        <v>0.45361808916891094</v>
       </c>
     </row>
     <row r="56">
@@ -854,13 +866,13 @@
         <v>4.5</v>
       </c>
       <c r="B56" s="0">
-        <v>3.3999999999999999</v>
+        <v>3.7999999999999998</v>
       </c>
       <c r="C56" s="0">
-        <v>1.0513572054694857</v>
+        <v>1.4677913845542852</v>
       </c>
       <c r="D56" s="0">
-        <v>0.44740791942472491</v>
+        <v>0.44740791942472496</v>
       </c>
     </row>
     <row r="57">
@@ -868,10 +880,10 @@
         <v>5</v>
       </c>
       <c r="B57" s="0">
-        <v>3.3999999999999999</v>
+        <v>3.7999999999999998</v>
       </c>
       <c r="C57" s="0">
-        <v>1.0304514092262784</v>
+        <v>1.4386049696484924</v>
       </c>
       <c r="D57" s="0">
         <v>0.43851140095085966</v>
@@ -882,13 +894,13 @@
         <v>5.5</v>
       </c>
       <c r="B58" s="0">
-        <v>3.3999999999999999</v>
+        <v>3.7999999999999998</v>
       </c>
       <c r="C58" s="0">
-        <v>1.0073466108969198</v>
+        <v>1.406348545520451</v>
       </c>
       <c r="D58" s="0">
-        <v>0.42867909115596925</v>
+        <v>0.42867909115596947</v>
       </c>
     </row>
     <row r="59">
@@ -896,13 +908,13 @@
         <v>6</v>
       </c>
       <c r="B59" s="0">
-        <v>3.3999999999999999</v>
+        <v>3.7999999999999998</v>
       </c>
       <c r="C59" s="0">
-        <v>0.98391391755805047</v>
+        <v>1.3736343497925236</v>
       </c>
       <c r="D59" s="0">
-        <v>0.41870724474761228</v>
+        <v>0.41870724474761234</v>
       </c>
     </row>
     <row r="60">
@@ -910,10 +922,10 @@
         <v>6.5</v>
       </c>
       <c r="B60" s="0">
-        <v>3.3999999999999999</v>
+        <v>3.7999999999999998</v>
       </c>
       <c r="C60" s="0">
-        <v>0.9607021516341</v>
+        <v>1.3412285890613254</v>
       </c>
       <c r="D60" s="0">
         <v>0.40882941460179528</v>
@@ -924,10 +936,10 @@
         <v>7</v>
       </c>
       <c r="B61" s="0">
-        <v>3.3999999999999999</v>
+        <v>3.7999999999999998</v>
       </c>
       <c r="C61" s="0">
-        <v>0.93694034686108651</v>
+        <v>1.3080549234928134</v>
       </c>
       <c r="D61" s="0">
         <v>0.39871751392715915</v>
@@ -938,13 +950,13 @@
         <v>7.5</v>
       </c>
       <c r="B62" s="0">
-        <v>3.3999999999999999</v>
+        <v>3.7999999999999998</v>
       </c>
       <c r="C62" s="0">
-        <v>0.94948383177279472</v>
+        <v>1.3255667824403825</v>
       </c>
       <c r="D62" s="0">
-        <v>0.40405542806089706</v>
+        <v>0.40405542806089711</v>
       </c>
     </row>
     <row r="63">
@@ -952,10 +964,10 @@
         <v>8</v>
       </c>
       <c r="B63" s="0">
-        <v>3.3999999999999999</v>
+        <v>3.7999999999999998</v>
       </c>
       <c r="C63" s="0">
-        <v>0.92591554690165301</v>
+        <v>1.2926632884588718</v>
       </c>
       <c r="D63" s="0">
         <v>0.39402588030705066</v>
@@ -966,13 +978,13 @@
         <v>8.5</v>
       </c>
       <c r="B64" s="0">
-        <v>3.3999999999999999</v>
+        <v>3.7999999999999998</v>
       </c>
       <c r="C64" s="0">
-        <v>0.90220904371418731</v>
+        <v>1.2595668289915758</v>
       </c>
       <c r="D64" s="0">
-        <v>0.38393751337261439</v>
+        <v>0.3839375133726145</v>
       </c>
     </row>
     <row r="65">
@@ -980,10 +992,10 @@
         <v>9</v>
       </c>
       <c r="B65" s="0">
-        <v>3.3999999999999999</v>
+        <v>3.7999999999999998</v>
       </c>
       <c r="C65" s="0">
-        <v>0.87817523824292121</v>
+        <v>1.2260134254240171</v>
       </c>
       <c r="D65" s="0">
         <v>0.37370986206075035</v>
@@ -994,13 +1006,13 @@
         <v>9.5</v>
       </c>
       <c r="B66" s="0">
-        <v>3.3999999999999999</v>
+        <v>3.7999999999999998</v>
       </c>
       <c r="C66" s="0">
-        <v>0.85351610050058035</v>
+        <v>1.1915870004749602</v>
       </c>
       <c r="D66" s="0">
-        <v>0.36321609889946421</v>
+        <v>0.36321609889946416</v>
       </c>
     </row>
     <row r="67">
@@ -1008,13 +1020,13 @@
         <v>10</v>
       </c>
       <c r="B67" s="0">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="C67" s="0">
-        <v>0.90376794364976321</v>
+        <v>1.3490646855646609</v>
       </c>
       <c r="D67" s="0">
-        <v>0.35256802490180772</v>
+        <v>0.35256802490180766</v>
       </c>
     </row>
     <row r="68">
@@ -1022,13 +1034,13 @@
         <v>4</v>
       </c>
       <c r="B68" s="0">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="C68" s="0">
-        <v>1.1627982650006314</v>
+        <v>1.7357221914878229</v>
       </c>
       <c r="D68" s="0">
-        <v>0.45361808916891083</v>
+        <v>0.45361808916891078</v>
       </c>
     </row>
     <row r="69">
@@ -1036,13 +1048,13 @@
         <v>4.5</v>
       </c>
       <c r="B69" s="0">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="C69" s="0">
-        <v>1.1468792027402863</v>
+        <v>1.7119596262478909</v>
       </c>
       <c r="D69" s="0">
-        <v>0.44740791942472502</v>
+        <v>0.44740791942472496</v>
       </c>
     </row>
     <row r="70">
@@ -1050,10 +1062,10 @@
         <v>5</v>
       </c>
       <c r="B70" s="0">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="C70" s="0">
-        <v>1.1240739917203513</v>
+        <v>1.6779180284572008</v>
       </c>
       <c r="D70" s="0">
         <v>0.43851140095085961</v>
@@ -1064,10 +1076,10 @@
         <v>5.5</v>
       </c>
       <c r="B71" s="0">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="C71" s="0">
-        <v>1.098869986317053</v>
+        <v>1.6402957230155428</v>
       </c>
       <c r="D71" s="0">
         <v>0.42867909115596942</v>
@@ -1078,10 +1090,10 @@
         <v>6</v>
       </c>
       <c r="B72" s="0">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="C72" s="0">
-        <v>1.0733082947104979</v>
+        <v>1.6021394953112973</v>
       </c>
       <c r="D72" s="0">
         <v>0.41870724474761223</v>
@@ -1092,13 +1104,13 @@
         <v>6.5</v>
       </c>
       <c r="B73" s="0">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="C73" s="0">
-        <v>1.0479876030763291</v>
+        <v>1.5643430110060654</v>
       </c>
       <c r="D73" s="0">
-        <v>0.40882941460179528</v>
+        <v>0.40882941460179523</v>
       </c>
     </row>
     <row r="74">
@@ -1106,13 +1118,13 @@
         <v>7</v>
       </c>
       <c r="B74" s="0">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="C74" s="0">
-        <v>1.0220668983225392</v>
+        <v>1.5256508802948694</v>
       </c>
       <c r="D74" s="0">
-        <v>0.3987175139271591</v>
+        <v>0.39871751392715915</v>
       </c>
     </row>
     <row r="75">
@@ -1120,13 +1132,13 @@
         <v>7.5</v>
       </c>
       <c r="B75" s="0">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="C75" s="0">
-        <v>1.0357500327513376</v>
+        <v>1.5460758506375654</v>
       </c>
       <c r="D75" s="0">
-        <v>0.40405542806089706</v>
+        <v>0.40405542806089711</v>
       </c>
     </row>
     <row r="76">
@@ -1134,10 +1146,10 @@
         <v>8</v>
       </c>
       <c r="B76" s="0">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="C76" s="0">
-        <v>1.0100404303228265</v>
+        <v>1.5076988347676012</v>
       </c>
       <c r="D76" s="0">
         <v>0.39402588030705066</v>
@@ -1148,13 +1160,13 @@
         <v>8.5</v>
       </c>
       <c r="B77" s="0">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="C77" s="0">
-        <v>0.98418005162949795</v>
+        <v>1.4690967534527779</v>
       </c>
       <c r="D77" s="0">
-        <v>0.3839375133726145</v>
+        <v>0.38393751337261434</v>
       </c>
     </row>
     <row r="78">
@@ -1162,10 +1174,10 @@
         <v>9</v>
       </c>
       <c r="B78" s="0">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="C78" s="0">
-        <v>0.95796263331124709</v>
+        <v>1.4299617150301998</v>
       </c>
       <c r="D78" s="0">
         <v>0.37370986206075041</v>
@@ -1176,10 +1188,10 @@
         <v>9.5</v>
       </c>
       <c r="B79" s="0">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="C79" s="0">
-        <v>0.93106306760030477</v>
+        <v>1.3898084274383558</v>
       </c>
       <c r="D79" s="0">
         <v>0.36321609889946416</v>
@@ -1190,13 +1202,13 @@
         <v>10</v>
       </c>
       <c r="B80" s="0">
-        <v>3.6000000000000001</v>
+        <v>4.2000000000000002</v>
       </c>
       <c r="C80" s="0">
-        <v>0.9834681557766376</v>
+        <v>1.5617110066267903</v>
       </c>
       <c r="D80" s="0">
-        <v>0.3525680249018075</v>
+        <v>0.35256802490180755</v>
       </c>
     </row>
     <row r="81">
@@ -1204,13 +1216,13 @@
         <v>4</v>
       </c>
       <c r="B81" s="0">
-        <v>3.6000000000000001</v>
+        <v>4.2000000000000002</v>
       </c>
       <c r="C81" s="0">
-        <v>1.2653414775946232</v>
+        <v>2.009315401921091</v>
       </c>
       <c r="D81" s="0">
-        <v>0.45361808916891078</v>
+        <v>0.45361808916891067</v>
       </c>
     </row>
     <row r="82">
@@ -1218,13 +1230,13 @@
         <v>4.5</v>
       </c>
       <c r="B82" s="0">
-        <v>3.6000000000000001</v>
+        <v>4.2000000000000002</v>
       </c>
       <c r="C82" s="0">
-        <v>1.2480185675347124</v>
+        <v>1.9818072623352148</v>
       </c>
       <c r="D82" s="0">
-        <v>0.44740791942472485</v>
+        <v>0.44740791942472491</v>
       </c>
     </row>
     <row r="83">
@@ -1232,13 +1244,13 @@
         <v>5</v>
       </c>
       <c r="B83" s="0">
-        <v>3.6000000000000001</v>
+        <v>4.2000000000000002</v>
       </c>
       <c r="C83" s="0">
-        <v>1.2232022427452993</v>
+        <v>1.9423998576927672</v>
       </c>
       <c r="D83" s="0">
-        <v>0.4385114009508595</v>
+        <v>0.43851140095085955</v>
       </c>
     </row>
     <row r="84">
@@ -1246,13 +1258,13 @@
         <v>5.5</v>
       </c>
       <c r="B84" s="0">
-        <v>3.6000000000000001</v>
+        <v>4.2000000000000002</v>
       </c>
       <c r="C84" s="0">
-        <v>1.1957755820783305</v>
+        <v>1.8988473363558676</v>
       </c>
       <c r="D84" s="0">
-        <v>0.42867909115596925</v>
+        <v>0.42867909115596931</v>
       </c>
     </row>
     <row r="85">
@@ -1260,13 +1272,13 @@
         <v>6</v>
       </c>
       <c r="B85" s="0">
-        <v>3.6000000000000001</v>
+        <v>4.2000000000000002</v>
       </c>
       <c r="C85" s="0">
-        <v>1.1679596920819357</v>
+        <v>1.8546767332597409</v>
       </c>
       <c r="D85" s="0">
-        <v>0.41870724474761217</v>
+        <v>0.41870724474761223</v>
       </c>
     </row>
     <row r="86">
@@ -1274,13 +1286,13 @@
         <v>6.5</v>
       </c>
       <c r="B86" s="0">
-        <v>3.6000000000000001</v>
+        <v>4.2000000000000002</v>
       </c>
       <c r="C86" s="0">
-        <v>1.1404060550234221</v>
+        <v>1.8109225781158969</v>
       </c>
       <c r="D86" s="0">
-        <v>0.40882941460179528</v>
+        <v>0.40882941460179523</v>
       </c>
     </row>
     <row r="87">
@@ -1288,10 +1300,10 @@
         <v>7</v>
       </c>
       <c r="B87" s="0">
-        <v>3.6000000000000001</v>
+        <v>4.2000000000000002</v>
       </c>
       <c r="C87" s="0">
-        <v>1.1121994917349598</v>
+        <v>1.7661316003013481</v>
       </c>
       <c r="D87" s="0">
         <v>0.3987175139271591</v>
@@ -1302,10 +1314,10 @@
         <v>7.5</v>
       </c>
       <c r="B88" s="0">
-        <v>3.6000000000000001</v>
+        <v>4.2000000000000002</v>
       </c>
       <c r="C88" s="0">
-        <v>1.1270892951147851</v>
+        <v>1.7897760565943115</v>
       </c>
       <c r="D88" s="0">
         <v>0.404055428060897</v>
@@ -1316,13 +1328,13 @@
         <v>8</v>
       </c>
       <c r="B89" s="0">
-        <v>3.6000000000000001</v>
+        <v>4.2000000000000002</v>
       </c>
       <c r="C89" s="0">
-        <v>1.0991124505455814</v>
+        <v>1.7453498635978442</v>
       </c>
       <c r="D89" s="0">
-        <v>0.3940258803070506</v>
+        <v>0.39402588030705055</v>
       </c>
     </row>
     <row r="90">
@@ -1330,13 +1342,13 @@
         <v>8.5</v>
       </c>
       <c r="B90" s="0">
-        <v>3.6000000000000001</v>
+        <v>4.2000000000000002</v>
       </c>
       <c r="C90" s="0">
-        <v>1.0709715332670755</v>
+        <v>1.7006631292157723</v>
       </c>
       <c r="D90" s="0">
-        <v>0.38393751337261445</v>
+        <v>0.38393751337261439</v>
       </c>
     </row>
     <row r="91">
@@ -1344,13 +1356,13 @@
         <v>9</v>
       </c>
       <c r="B91" s="0">
-        <v>3.6000000000000001</v>
+        <v>4.2000000000000002</v>
       </c>
       <c r="C91" s="0">
-        <v>1.0424420902570155</v>
+        <v>1.6553594303618353</v>
       </c>
       <c r="D91" s="0">
-        <v>0.3737098620607503</v>
+        <v>0.37370986206075041</v>
       </c>
     </row>
     <row r="92">
@@ -1358,13 +1370,13 @@
         <v>9.5</v>
       </c>
       <c r="B92" s="0">
-        <v>3.6000000000000001</v>
+        <v>4.2000000000000002</v>
       </c>
       <c r="C92" s="0">
-        <v>1.0131703436025616</v>
+        <v>1.6088769808133268</v>
       </c>
       <c r="D92" s="0">
-        <v>0.36321609889946416</v>
+        <v>0.3632160988994641</v>
       </c>
     </row>
     <row r="93">
@@ -1372,13 +1384,13 @@
         <v>10</v>
       </c>
       <c r="B93" s="0">
-        <v>3.7000000000000002</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C93" s="0">
-        <v>1.0677214612172932</v>
+        <v>1.7956050964865626</v>
       </c>
       <c r="D93" s="0">
-        <v>0.35256802490180761</v>
+        <v>0.35256802490180739</v>
       </c>
     </row>
     <row r="94">
@@ -1386,13 +1398,13 @@
         <v>4</v>
       </c>
       <c r="B94" s="0">
-        <v>3.7000000000000002</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C94" s="0">
-        <v>1.373742752584886</v>
+        <v>2.3102462368702921</v>
       </c>
       <c r="D94" s="0">
-        <v>0.45361808916891078</v>
+        <v>0.45361808916891061</v>
       </c>
     </row>
     <row r="95">
@@ -1400,13 +1412,13 @@
         <v>4.5</v>
       </c>
       <c r="B95" s="0">
-        <v>3.7000000000000002</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C95" s="0">
-        <v>1.3549357960677251</v>
+        <v>2.2786182625359421</v>
       </c>
       <c r="D95" s="0">
-        <v>0.44740791942472485</v>
+        <v>0.44740791942472474</v>
       </c>
     </row>
     <row r="96">
@@ -1414,13 +1426,13 @@
         <v>5</v>
       </c>
       <c r="B96" s="0">
-        <v>3.7000000000000002</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C96" s="0">
-        <v>1.3279934671162907</v>
+        <v>2.2333088958765335</v>
       </c>
       <c r="D96" s="0">
-        <v>0.43851140095085966</v>
+        <v>0.43851140095085939</v>
       </c>
     </row>
     <row r="97">
@@ -1428,13 +1440,13 @@
         <v>5.5</v>
       </c>
       <c r="B97" s="0">
-        <v>3.7000000000000002</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C97" s="0">
-        <v>1.2982171759047858</v>
+        <v>2.183233607333686</v>
       </c>
       <c r="D97" s="0">
-        <v>0.42867909115596942</v>
+        <v>0.42867909115596903</v>
       </c>
     </row>
     <row r="98">
@@ -1442,13 +1454,13 @@
         <v>6</v>
       </c>
       <c r="B98" s="0">
-        <v>3.7000000000000002</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C98" s="0">
-        <v>1.2680183102500493</v>
+        <v>2.1324476682593358</v>
       </c>
       <c r="D98" s="0">
-        <v>0.41870724474761228</v>
+        <v>0.41870724474761201</v>
       </c>
     </row>
     <row r="99">
@@ -1456,13 +1468,13 @@
         <v>6.5</v>
       </c>
       <c r="B99" s="0">
-        <v>3.7000000000000002</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C99" s="0">
-        <v>1.23810416463266</v>
+        <v>2.0821405476490726</v>
       </c>
       <c r="D99" s="0">
-        <v>0.40882941460179523</v>
+        <v>0.40882941460179506</v>
       </c>
     </row>
     <row r="100">
@@ -1470,13 +1482,13 @@
         <v>7</v>
       </c>
       <c r="B100" s="0">
-        <v>3.7000000000000002</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C100" s="0">
-        <v>1.207481156868375</v>
+        <v>2.0306413216724706</v>
       </c>
       <c r="D100" s="0">
-        <v>0.39871751392715904</v>
+        <v>0.39871751392715898</v>
       </c>
     </row>
     <row r="101">
@@ -1484,13 +1496,13 @@
         <v>7.5</v>
       </c>
       <c r="B101" s="0">
-        <v>3.7000000000000002</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C101" s="0">
-        <v>1.223646563474134</v>
+        <v>2.0578269571985981</v>
       </c>
       <c r="D101" s="0">
-        <v>0.40405542806089695</v>
+        <v>0.40405542806089673</v>
       </c>
     </row>
     <row r="102">
@@ -1498,13 +1510,13 @@
         <v>8</v>
       </c>
       <c r="B102" s="0">
-        <v>3.7000000000000002</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C102" s="0">
-        <v>1.1932729543356764</v>
+        <v>2.0067471490756761</v>
       </c>
       <c r="D102" s="0">
-        <v>0.39402588030705055</v>
+        <v>0.39402588030705038</v>
       </c>
     </row>
     <row r="103">
@@ -1512,13 +1524,13 @@
         <v>8.5</v>
       </c>
       <c r="B103" s="0">
-        <v>3.7000000000000002</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C103" s="0">
-        <v>1.162721216447556</v>
+        <v>1.9553677788456472</v>
       </c>
       <c r="D103" s="0">
-        <v>0.38393751337261445</v>
+        <v>0.38393751337261423</v>
       </c>
     </row>
     <row r="104">
@@ -1526,13 +1538,13 @@
         <v>9</v>
       </c>
       <c r="B104" s="0">
-        <v>3.7000000000000002</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C104" s="0">
-        <v>1.1317476679910112</v>
+        <v>1.9032790427051951</v>
       </c>
       <c r="D104" s="0">
-        <v>0.37370986206075046</v>
+        <v>0.37370986206075019</v>
       </c>
     </row>
     <row r="105">
@@ -1540,13 +1552,13 @@
         <v>9.5</v>
       </c>
       <c r="B105" s="0">
-        <v>3.7000000000000002</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C105" s="0">
-        <v>1.0999682230474226</v>
+        <v>1.8498350169204512</v>
       </c>
       <c r="D105" s="0">
-        <v>0.36321609889946416</v>
+        <v>0.36321609889946399</v>
       </c>
     </row>
     <row r="106">
@@ -1554,13 +1566,13 @@
         <v>10</v>
       </c>
       <c r="B106" s="0">
-        <v>3.7999999999999998</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C106" s="0">
-        <v>1.156654334786001</v>
+        <v>2.0517587536581541</v>
       </c>
       <c r="D106" s="0">
-        <v>0.35256802490180766</v>
+        <v>0.35256802490180783</v>
       </c>
     </row>
     <row r="107">
@@ -1568,10 +1580,10 @@
         <v>4</v>
       </c>
       <c r="B107" s="0">
-        <v>3.7999999999999998</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C107" s="0">
-        <v>1.4881648139268726</v>
+        <v>2.6398164879790431</v>
       </c>
       <c r="D107" s="0">
         <v>0.45361808916891094</v>
@@ -1582,13 +1594,13 @@
         <v>4.5</v>
       </c>
       <c r="B108" s="0">
-        <v>3.7999999999999998</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C108" s="0">
-        <v>1.4677913845542852</v>
+        <v>2.6036765965697612</v>
       </c>
       <c r="D108" s="0">
-        <v>0.44740791942472496</v>
+        <v>0.44740791942472508</v>
       </c>
     </row>
     <row r="109">
@@ -1596,13 +1608,13 @@
         <v>5</v>
       </c>
       <c r="B109" s="0">
-        <v>3.7999999999999998</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C109" s="0">
-        <v>1.4386049696484924</v>
+        <v>2.5519035815298454</v>
       </c>
       <c r="D109" s="0">
-        <v>0.43851140095085966</v>
+        <v>0.43851140095085972</v>
       </c>
     </row>
     <row r="110">
@@ -1610,13 +1622,13 @@
         <v>5.5</v>
       </c>
       <c r="B110" s="0">
-        <v>3.7999999999999998</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C110" s="0">
-        <v>1.406348545520451</v>
+        <v>2.4946847577412639</v>
       </c>
       <c r="D110" s="0">
-        <v>0.42867909115596947</v>
+        <v>0.42867909115596953</v>
       </c>
     </row>
     <row r="111">
@@ -1624,10 +1636,10 @@
         <v>6</v>
       </c>
       <c r="B111" s="0">
-        <v>3.7999999999999998</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C111" s="0">
-        <v>1.3736343497925236</v>
+        <v>2.4366539049315694</v>
       </c>
       <c r="D111" s="0">
         <v>0.41870724474761234</v>
@@ -1638,13 +1650,13 @@
         <v>6.5</v>
       </c>
       <c r="B112" s="0">
-        <v>3.7999999999999998</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C112" s="0">
-        <v>1.3412285890613254</v>
+        <v>2.3791701768638505</v>
       </c>
       <c r="D112" s="0">
-        <v>0.40882941460179528</v>
+        <v>0.40882941460179539</v>
       </c>
     </row>
     <row r="113">
@@ -1652,13 +1664,13 @@
         <v>7</v>
       </c>
       <c r="B113" s="0">
-        <v>3.7999999999999998</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C113" s="0">
-        <v>1.3080549234928134</v>
+        <v>2.3203242825684596</v>
       </c>
       <c r="D113" s="0">
-        <v>0.39871751392715915</v>
+        <v>0.39871751392715926</v>
       </c>
     </row>
     <row r="114">
@@ -1666,13 +1678,13 @@
         <v>7.5</v>
       </c>
       <c r="B114" s="0">
-        <v>3.7999999999999998</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C114" s="0">
-        <v>1.3255667824403825</v>
+        <v>2.3513881093384077</v>
       </c>
       <c r="D114" s="0">
-        <v>0.40405542806089711</v>
+        <v>0.40405542806089728</v>
       </c>
     </row>
     <row r="115">
@@ -1680,13 +1692,13 @@
         <v>8</v>
       </c>
       <c r="B115" s="0">
-        <v>3.7999999999999998</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C115" s="0">
-        <v>1.2926632884588718</v>
+        <v>2.2930214653271759</v>
       </c>
       <c r="D115" s="0">
-        <v>0.39402588030705066</v>
+        <v>0.39402588030705082</v>
       </c>
     </row>
     <row r="116">
@@ -1694,13 +1706,13 @@
         <v>8.5</v>
       </c>
       <c r="B116" s="0">
-        <v>3.7999999999999998</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C116" s="0">
-        <v>1.2595668289915758</v>
+        <v>2.2343125249074944</v>
       </c>
       <c r="D116" s="0">
-        <v>0.3839375133726145</v>
+        <v>0.38393751337261461</v>
       </c>
     </row>
     <row r="117">
@@ -1708,13 +1720,13 @@
         <v>9</v>
       </c>
       <c r="B117" s="0">
-        <v>3.7999999999999998</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C117" s="0">
-        <v>1.2260134254240171</v>
+        <v>2.1747930233465556</v>
       </c>
       <c r="D117" s="0">
-        <v>0.37370986206075035</v>
+        <v>0.37370986206075058</v>
       </c>
     </row>
     <row r="118">
@@ -1722,13 +1734,13 @@
         <v>9.5</v>
       </c>
       <c r="B118" s="0">
-        <v>3.7999999999999998</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C118" s="0">
-        <v>1.1915870004749602</v>
+        <v>2.11372489208031</v>
       </c>
       <c r="D118" s="0">
-        <v>0.36321609889946416</v>
+        <v>0.36321609889946432</v>
       </c>
     </row>
     <row r="119">
@@ -1736,13 +1748,13 @@
         <v>10</v>
       </c>
       <c r="B119" s="0">
-        <v>3.8999999999999999</v>
+        <v>4.7999999999999998</v>
       </c>
       <c r="C119" s="0">
-        <v>1.2503932512970326</v>
+        <v>2.3311837766557346</v>
       </c>
       <c r="D119" s="0">
-        <v>0.35256802490180755</v>
+        <v>0.35256802490180777</v>
       </c>
     </row>
     <row r="120">
@@ -1750,13 +1762,13 @@
         <v>4</v>
       </c>
       <c r="B120" s="0">
-        <v>3.8999999999999999</v>
+        <v>4.7999999999999998</v>
       </c>
       <c r="C120" s="0">
-        <v>1.6087703855760336</v>
+        <v>2.9993279468909586</v>
       </c>
       <c r="D120" s="0">
-        <v>0.45361808916891072</v>
+        <v>0.45361808916891089</v>
       </c>
     </row>
     <row r="121">
@@ -1764,13 +1776,13 @@
         <v>4.5</v>
       </c>
       <c r="B121" s="0">
-        <v>3.8999999999999999</v>
+        <v>4.7999999999999998</v>
       </c>
       <c r="C121" s="0">
-        <v>1.5867458292093535</v>
+        <v>2.9582662341563566</v>
       </c>
       <c r="D121" s="0">
-        <v>0.44740791942472491</v>
+        <v>0.44740791942472519</v>
       </c>
     </row>
     <row r="122">
@@ -1778,13 +1790,13 @@
         <v>5</v>
       </c>
       <c r="B122" s="0">
-        <v>3.8999999999999999</v>
+        <v>4.7999999999999998</v>
       </c>
       <c r="C122" s="0">
-        <v>1.5551940551570729</v>
+        <v>2.8994423531740434</v>
       </c>
       <c r="D122" s="0">
-        <v>0.4385114009508595</v>
+        <v>0.43851140095085972</v>
       </c>
     </row>
     <row r="123">
@@ -1792,13 +1804,13 @@
         <v>5.5</v>
       </c>
       <c r="B123" s="0">
-        <v>3.8999999999999999</v>
+        <v>4.7999999999999998</v>
       </c>
       <c r="C123" s="0">
-        <v>1.5203234686493583</v>
+        <v>2.8344310093708582</v>
       </c>
       <c r="D123" s="0">
-        <v>0.42867909115596919</v>
+        <v>0.42867909115596953</v>
       </c>
     </row>
     <row r="124">
@@ -1806,13 +1818,13 @@
         <v>6</v>
       </c>
       <c r="B124" s="0">
-        <v>3.8999999999999999</v>
+        <v>4.7999999999999998</v>
       </c>
       <c r="C124" s="0">
-        <v>1.484958011287044</v>
+        <v>2.7684970478979229</v>
       </c>
       <c r="D124" s="0">
-        <v>0.41870724474761212</v>
+        <v>0.41870724474761245</v>
       </c>
     </row>
     <row r="125">
@@ -1820,13 +1832,13 @@
         <v>6.5</v>
       </c>
       <c r="B125" s="0">
-        <v>3.8999999999999999</v>
+        <v>4.7999999999999998</v>
       </c>
       <c r="C125" s="0">
-        <v>1.4499259854666999</v>
+        <v>2.7031847230184822</v>
       </c>
       <c r="D125" s="0">
-        <v>0.40882941460179523</v>
+        <v>0.40882941460179545</v>
       </c>
     </row>
     <row r="126">
@@ -1834,13 +1846,13 @@
         <v>7</v>
       </c>
       <c r="B126" s="0">
-        <v>3.8999999999999999</v>
+        <v>4.7999999999999998</v>
       </c>
       <c r="C126" s="0">
-        <v>1.4140638213783019</v>
+        <v>2.6363247211495349</v>
       </c>
       <c r="D126" s="0">
-        <v>0.39871751392715904</v>
+        <v>0.39871751392715932</v>
       </c>
     </row>
     <row r="127">
@@ -1848,13 +1860,13 @@
         <v>7.5</v>
       </c>
       <c r="B127" s="0">
-        <v>3.8999999999999999</v>
+        <v>4.7999999999999998</v>
       </c>
       <c r="C127" s="0">
-        <v>1.4329948966245267</v>
+        <v>2.6716190699017131</v>
       </c>
       <c r="D127" s="0">
-        <v>0.404055428060897</v>
+        <v>0.40405542806089717</v>
       </c>
     </row>
     <row r="128">
@@ -1862,13 +1874,13 @@
         <v>8</v>
       </c>
       <c r="B128" s="0">
-        <v>3.8999999999999999</v>
+        <v>4.7999999999999998</v>
       </c>
       <c r="C128" s="0">
-        <v>1.3974247996809266</v>
+        <v>2.6053035864784158</v>
       </c>
       <c r="D128" s="0">
-        <v>0.39402588030705055</v>
+        <v>0.39402588030705082</v>
       </c>
     </row>
     <row r="129">
@@ -1876,13 +1888,13 @@
         <v>8.5</v>
       </c>
       <c r="B129" s="0">
-        <v>3.8999999999999999</v>
+        <v>4.7999999999999998</v>
       </c>
       <c r="C129" s="0">
-        <v>1.3616460987197707</v>
+        <v>2.5385991899664013</v>
       </c>
       <c r="D129" s="0">
-        <v>0.38393751337261434</v>
+        <v>0.38393751337261456</v>
       </c>
     </row>
     <row r="130">
@@ -1890,13 +1902,13 @@
         <v>9</v>
       </c>
       <c r="B130" s="0">
-        <v>3.8999999999999999</v>
+        <v>4.7999999999999998</v>
       </c>
       <c r="C130" s="0">
-        <v>1.3253734214668187</v>
+        <v>2.4709738435721857</v>
       </c>
       <c r="D130" s="0">
-        <v>0.37370986206075035</v>
+        <v>0.37370986206075052</v>
       </c>
     </row>
     <row r="131">
@@ -1904,13 +1916,13 @@
         <v>9.5</v>
       </c>
       <c r="B131" s="0">
-        <v>3.8999999999999999</v>
+        <v>4.7999999999999998</v>
       </c>
       <c r="C131" s="0">
-        <v>1.2881569704252469</v>
+        <v>2.4015889626134799</v>
       </c>
       <c r="D131" s="0">
-        <v>0.36321609889946405</v>
+        <v>0.36321609889946432</v>
       </c>
     </row>
     <row r="132">
@@ -1918,13 +1930,13 @@
         <v>10</v>
       </c>
       <c r="B132" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C132" s="0">
-        <v>1.3490646855646609</v>
+        <v>2.6348919639934776</v>
       </c>
       <c r="D132" s="0">
-        <v>0.35256802490180766</v>
+        <v>0.35256802490180755</v>
       </c>
     </row>
     <row r="133">
@@ -1932,10 +1944,10 @@
         <v>4</v>
       </c>
       <c r="B133" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C133" s="0">
-        <v>1.7357221914878229</v>
+        <v>3.3900824052496543</v>
       </c>
       <c r="D133" s="0">
         <v>0.45361808916891078</v>
@@ -1946,13 +1958,13 @@
         <v>4.5</v>
       </c>
       <c r="B134" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C134" s="0">
-        <v>1.7119596262478909</v>
+        <v>3.3436711450154113</v>
       </c>
       <c r="D134" s="0">
-        <v>0.44740791942472496</v>
+        <v>0.44740791942472491</v>
       </c>
     </row>
     <row r="135">
@@ -1960,10 +1972,10 @@
         <v>5</v>
       </c>
       <c r="B135" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C135" s="0">
-        <v>1.6779180284572008</v>
+        <v>3.2771836493304702</v>
       </c>
       <c r="D135" s="0">
         <v>0.43851140095085961</v>
@@ -1974,13 +1986,13 @@
         <v>5.5</v>
       </c>
       <c r="B136" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C136" s="0">
-        <v>1.6402957230155428</v>
+        <v>3.2037025840147311</v>
       </c>
       <c r="D136" s="0">
-        <v>0.42867909115596942</v>
+        <v>0.42867909115596931</v>
       </c>
     </row>
     <row r="137">
@@ -1988,10 +2000,10 @@
         <v>6</v>
       </c>
       <c r="B137" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C137" s="0">
-        <v>1.6021394953112973</v>
+        <v>3.1291787017798773</v>
       </c>
       <c r="D137" s="0">
         <v>0.41870724474761223</v>
@@ -2002,10 +2014,10 @@
         <v>6.5</v>
       </c>
       <c r="B138" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C138" s="0">
-        <v>1.5643430110060654</v>
+        <v>3.0553574433712214</v>
       </c>
       <c r="D138" s="0">
         <v>0.40882941460179523</v>
@@ -2016,13 +2028,13 @@
         <v>7</v>
       </c>
       <c r="B139" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C139" s="0">
-        <v>1.5256508802948694</v>
+        <v>2.979786875575916</v>
       </c>
       <c r="D139" s="0">
-        <v>0.39871751392715915</v>
+        <v>0.3987175139271591</v>
       </c>
     </row>
     <row r="140">
@@ -2030,13 +2042,13 @@
         <v>7.5</v>
       </c>
       <c r="B140" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C140" s="0">
-        <v>1.5460758506375654</v>
+        <v>3.0196793957764942</v>
       </c>
       <c r="D140" s="0">
-        <v>0.40405542806089711</v>
+        <v>0.404055428060897</v>
       </c>
     </row>
     <row r="141">
@@ -2044,13 +2056,13 @@
         <v>8</v>
       </c>
       <c r="B141" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C141" s="0">
-        <v>1.5076988347676012</v>
+        <v>2.9447242866554704</v>
       </c>
       <c r="D141" s="0">
-        <v>0.39402588030705066</v>
+        <v>0.39402588030705055</v>
       </c>
     </row>
     <row r="142">
@@ -2058,13 +2070,13 @@
         <v>8.5</v>
       </c>
       <c r="B142" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C142" s="0">
-        <v>1.4690967534527779</v>
+        <v>2.8693295965874568</v>
       </c>
       <c r="D142" s="0">
-        <v>0.38393751337261434</v>
+        <v>0.38393751337261439</v>
       </c>
     </row>
     <row r="143">
@@ -2072,13 +2084,13 @@
         <v>9</v>
       </c>
       <c r="B143" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C143" s="0">
-        <v>1.4299617150301998</v>
+        <v>2.7928939746683583</v>
       </c>
       <c r="D143" s="0">
-        <v>0.37370986206075041</v>
+        <v>0.37370986206075035</v>
       </c>
     </row>
     <row r="144">
@@ -2086,13 +2098,13 @@
         <v>9.5</v>
       </c>
       <c r="B144" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C144" s="0">
-        <v>1.3898084274383558</v>
+        <v>2.7144695848405385</v>
       </c>
       <c r="D144" s="0">
-        <v>0.36321609889946416</v>
+        <v>0.3632160988994641</v>
       </c>
     </row>
     <row r="145">
@@ -2100,13 +2112,13 @@
         <v>10</v>
       </c>
       <c r="B145" s="0">
-        <v>4.0999999999999996</v>
+        <v>5.2000000000000002</v>
       </c>
       <c r="C145" s="0">
-        <v>1.4527951124031557</v>
+        <v>2.9638951141855596</v>
       </c>
       <c r="D145" s="0">
-        <v>0.35256802490180772</v>
+        <v>0.35256802490180761</v>
       </c>
     </row>
     <row r="146">
@@ -2114,13 +2126,13 @@
         <v>4</v>
       </c>
       <c r="B146" s="0">
-        <v>4.0999999999999996</v>
+        <v>5.2000000000000002</v>
       </c>
       <c r="C146" s="0">
-        <v>1.8691829556176909</v>
+        <v>3.8133816546987469</v>
       </c>
       <c r="D146" s="0">
-        <v>0.45361808916891083</v>
+        <v>0.45361808916891078</v>
       </c>
     </row>
     <row r="147">
@@ -2128,10 +2140,10 @@
         <v>4.5</v>
       </c>
       <c r="B147" s="0">
-        <v>4.0999999999999996</v>
+        <v>5.2000000000000002</v>
       </c>
       <c r="C147" s="0">
-        <v>1.8435932718848567</v>
+        <v>3.7611752988666156</v>
       </c>
       <c r="D147" s="0">
         <v>0.44740791942472491</v>
@@ -2142,13 +2154,13 @@
         <v>5</v>
       </c>
       <c r="B148" s="0">
-        <v>4.0999999999999996</v>
+        <v>5.2000000000000002</v>
       </c>
       <c r="C148" s="0">
-        <v>1.8069341943640422</v>
+        <v>3.68638590852047</v>
       </c>
       <c r="D148" s="0">
-        <v>0.43851140095085966</v>
+        <v>0.43851140095085961</v>
       </c>
     </row>
     <row r="149">
@@ -2156,13 +2168,13 @@
         <v>5.5</v>
       </c>
       <c r="B149" s="0">
-        <v>4.0999999999999996</v>
+        <v>5.2000000000000002</v>
       </c>
       <c r="C149" s="0">
-        <v>1.766419086343034</v>
+        <v>3.6037297034651465</v>
       </c>
       <c r="D149" s="0">
-        <v>0.42867909115596942</v>
+        <v>0.42867909115596931</v>
       </c>
     </row>
     <row r="150">
@@ -2170,13 +2182,13 @@
         <v>6</v>
       </c>
       <c r="B150" s="0">
-        <v>4.0999999999999996</v>
+        <v>5.2000000000000002</v>
       </c>
       <c r="C150" s="0">
-        <v>1.7253290024429671</v>
+        <v>3.5199004711989197</v>
       </c>
       <c r="D150" s="0">
-        <v>0.41870724474761228</v>
+        <v>0.41870724474761217</v>
       </c>
     </row>
     <row r="151">
@@ -2184,10 +2196,10 @@
         <v>6.5</v>
       </c>
       <c r="B151" s="0">
-        <v>4.0999999999999996</v>
+        <v>5.2000000000000002</v>
       </c>
       <c r="C151" s="0">
-        <v>1.6846263228367031</v>
+        <v>3.4368615951803259</v>
       </c>
       <c r="D151" s="0">
         <v>0.40882941460179523</v>
@@ -2198,13 +2210,13 @@
         <v>7</v>
       </c>
       <c r="B152" s="0">
-        <v>4.0999999999999996</v>
+        <v>5.2000000000000002</v>
       </c>
       <c r="C152" s="0">
-        <v>1.6429591300125415</v>
+        <v>3.3518549840078276</v>
       </c>
       <c r="D152" s="0">
-        <v>0.39871751392715915</v>
+        <v>0.3987175139271591</v>
       </c>
     </row>
     <row r="153">
@@ -2212,13 +2224,13 @@
         <v>7.5</v>
       </c>
       <c r="B153" s="0">
-        <v>4.0999999999999996</v>
+        <v>5.2000000000000002</v>
       </c>
       <c r="C153" s="0">
-        <v>1.6649545890904938</v>
+        <v>3.39672864385073</v>
       </c>
       <c r="D153" s="0">
-        <v>0.40405542806089711</v>
+        <v>0.404055428060897</v>
       </c>
     </row>
     <row r="154">
@@ -2226,13 +2238,13 @@
         <v>8</v>
       </c>
       <c r="B154" s="0">
-        <v>4.0999999999999996</v>
+        <v>5.2000000000000002</v>
       </c>
       <c r="C154" s="0">
-        <v>1.6236267404846529</v>
+        <v>3.3124143399844197</v>
       </c>
       <c r="D154" s="0">
-        <v>0.3940258803070506</v>
+        <v>0.39402588030705066</v>
       </c>
     </row>
     <row r="155">
@@ -2240,10 +2252,10 @@
         <v>8.5</v>
       </c>
       <c r="B155" s="0">
-        <v>4.0999999999999996</v>
+        <v>5.2000000000000002</v>
       </c>
       <c r="C155" s="0">
-        <v>1.5820565210112325</v>
+        <v>3.2276055673357531</v>
       </c>
       <c r="D155" s="0">
         <v>0.38393751337261439</v>
@@ -2254,13 +2266,13 @@
         <v>9</v>
       </c>
       <c r="B156" s="0">
-        <v>4.0999999999999996</v>
+        <v>5.2000000000000002</v>
       </c>
       <c r="C156" s="0">
-        <v>1.5399123650249431</v>
+        <v>3.1416258879213483</v>
       </c>
       <c r="D156" s="0">
-        <v>0.37370986206075041</v>
+        <v>0.37370986206075035</v>
       </c>
     </row>
     <row r="157">
@@ -2268,13 +2280,13 @@
         <v>9.5</v>
       </c>
       <c r="B157" s="0">
-        <v>4.0999999999999996</v>
+        <v>5.2000000000000002</v>
       </c>
       <c r="C157" s="0">
-        <v>1.4966716660543578</v>
+        <v>3.0534091150820677</v>
       </c>
       <c r="D157" s="0">
-        <v>0.36321609889946421</v>
+        <v>0.36321609889946416</v>
       </c>
     </row>
     <row r="158">
@@ -2282,13 +2294,13 @@
         <v>10</v>
       </c>
       <c r="B158" s="0">
-        <v>4.2000000000000002</v>
+        <v>5.4000000000000004</v>
       </c>
       <c r="C158" s="0">
-        <v>1.5617110066267903</v>
+        <v>3.3192050257461516</v>
       </c>
       <c r="D158" s="0">
-        <v>0.35256802490180755</v>
+        <v>0.3525680249018075</v>
       </c>
     </row>
     <row r="159">
@@ -2296,13 +2308,13 @@
         <v>4</v>
       </c>
       <c r="B159" s="0">
-        <v>4.2000000000000002</v>
+        <v>5.4000000000000004</v>
       </c>
       <c r="C159" s="0">
-        <v>2.009315401921091</v>
+        <v>4.2705274868818526</v>
       </c>
       <c r="D159" s="0">
-        <v>0.45361808916891067</v>
+        <v>0.45361808916891072</v>
       </c>
     </row>
     <row r="160">
@@ -2310,13 +2322,13 @@
         <v>4.5</v>
       </c>
       <c r="B160" s="0">
-        <v>4.2000000000000002</v>
+        <v>5.4000000000000004</v>
       </c>
       <c r="C160" s="0">
-        <v>1.9818072623352148</v>
+        <v>4.212062665429654</v>
       </c>
       <c r="D160" s="0">
-        <v>0.44740791942472491</v>
+        <v>0.44740791942472485</v>
       </c>
     </row>
     <row r="161">
@@ -2324,13 +2336,13 @@
         <v>5</v>
       </c>
       <c r="B161" s="0">
-        <v>4.2000000000000002</v>
+        <v>5.4000000000000004</v>
       </c>
       <c r="C161" s="0">
-        <v>1.9423998576927672</v>
+        <v>4.1283075692653863</v>
       </c>
       <c r="D161" s="0">
-        <v>0.43851140095085955</v>
+        <v>0.43851140095085966</v>
       </c>
     </row>
     <row r="162">
@@ -2338,10 +2350,10 @@
         <v>5.5</v>
       </c>
       <c r="B162" s="0">
-        <v>4.2000000000000002</v>
+        <v>5.4000000000000004</v>
       </c>
       <c r="C162" s="0">
-        <v>1.8988473363558676</v>
+        <v>4.0357425895143653</v>
       </c>
       <c r="D162" s="0">
         <v>0.42867909115596931</v>
@@ -2352,13 +2364,13 @@
         <v>6</v>
       </c>
       <c r="B163" s="0">
-        <v>4.2000000000000002</v>
+        <v>5.4000000000000004</v>
       </c>
       <c r="C163" s="0">
-        <v>1.8546767332597409</v>
+        <v>3.9418639607765331</v>
       </c>
       <c r="D163" s="0">
-        <v>0.41870724474761223</v>
+        <v>0.41870724474761217</v>
       </c>
     </row>
     <row r="164">
@@ -2366,13 +2378,13 @@
         <v>6.5</v>
       </c>
       <c r="B164" s="0">
-        <v>4.2000000000000002</v>
+        <v>5.4000000000000004</v>
       </c>
       <c r="C164" s="0">
-        <v>1.8109225781158969</v>
+        <v>3.8488704357040482</v>
       </c>
       <c r="D164" s="0">
-        <v>0.40882941460179523</v>
+        <v>0.40882941460179517</v>
       </c>
     </row>
     <row r="165">
@@ -2380,13 +2392,13 @@
         <v>7</v>
       </c>
       <c r="B165" s="0">
-        <v>4.2000000000000002</v>
+        <v>5.4000000000000004</v>
       </c>
       <c r="C165" s="0">
-        <v>1.7661316003013481</v>
+        <v>3.7536732846054885</v>
       </c>
       <c r="D165" s="0">
-        <v>0.3987175139271591</v>
+        <v>0.39871751392715904</v>
       </c>
     </row>
     <row r="166">
@@ -2394,13 +2406,13 @@
         <v>7.5</v>
       </c>
       <c r="B166" s="0">
-        <v>4.2000000000000002</v>
+        <v>5.4000000000000004</v>
       </c>
       <c r="C166" s="0">
-        <v>1.7897760565943115</v>
+        <v>3.8039263710123987</v>
       </c>
       <c r="D166" s="0">
-        <v>0.404055428060897</v>
+        <v>0.40405542806089695</v>
       </c>
     </row>
     <row r="167">
@@ -2408,13 +2420,13 @@
         <v>8</v>
       </c>
       <c r="B167" s="0">
-        <v>4.2000000000000002</v>
+        <v>5.4000000000000004</v>
       </c>
       <c r="C167" s="0">
-        <v>1.7453498635978442</v>
+        <v>3.7095045205913366</v>
       </c>
       <c r="D167" s="0">
-        <v>0.39402588030705055</v>
+        <v>0.3940258803070506</v>
       </c>
     </row>
     <row r="168">
@@ -2422,10 +2434,10 @@
         <v>8.5</v>
       </c>
       <c r="B168" s="0">
-        <v>4.2000000000000002</v>
+        <v>5.4000000000000004</v>
       </c>
       <c r="C168" s="0">
-        <v>1.7006631292157723</v>
+        <v>3.614528924776379</v>
       </c>
       <c r="D168" s="0">
         <v>0.38393751337261439</v>
@@ -2436,13 +2448,13 @@
         <v>9</v>
       </c>
       <c r="B169" s="0">
-        <v>4.2000000000000002</v>
+        <v>5.4000000000000004</v>
       </c>
       <c r="C169" s="0">
-        <v>1.6553594303618353</v>
+        <v>3.5182420546174273</v>
       </c>
       <c r="D169" s="0">
-        <v>0.37370986206075041</v>
+        <v>0.37370986206075035</v>
       </c>
     </row>
     <row r="170">
@@ -2450,10 +2462,10 @@
         <v>9.5</v>
       </c>
       <c r="B170" s="0">
-        <v>4.2000000000000002</v>
+        <v>5.4000000000000004</v>
       </c>
       <c r="C170" s="0">
-        <v>1.6088769808133268</v>
+        <v>3.4194499096586446</v>
       </c>
       <c r="D170" s="0">
         <v>0.3632160988994641</v>
@@ -2464,13 +2476,13 @@
         <v>10</v>
       </c>
       <c r="B171" s="0">
-        <v>4.2999999999999998</v>
+        <v>5.5999999999999996</v>
       </c>
       <c r="C171" s="0">
-        <v>1.6759388430498352</v>
+        <v>3.7018334975200866</v>
       </c>
       <c r="D171" s="0">
-        <v>0.35256802490180755</v>
+        <v>0.35256802493329997</v>
       </c>
     </row>
     <row r="172">
@@ -2478,13 +2490,13 @@
         <v>4</v>
       </c>
       <c r="B172" s="0">
-        <v>4.2999999999999998</v>
+        <v>5.5999999999999996</v>
       </c>
       <c r="C172" s="0">
-        <v>2.1562822543534734</v>
+        <v>4.7628216934425858</v>
       </c>
       <c r="D172" s="0">
-        <v>0.45361808916891067</v>
+        <v>0.45361808916891083</v>
       </c>
     </row>
     <row r="173">
@@ -2492,13 +2504,13 @@
         <v>4.5</v>
       </c>
       <c r="B173" s="0">
-        <v>4.2999999999999998</v>
+        <v>5.5999999999999996</v>
       </c>
       <c r="C173" s="0">
-        <v>2.1267620938139222</v>
+        <v>4.6976172144242119</v>
       </c>
       <c r="D173" s="0">
-        <v>0.44740791942472491</v>
+        <v>0.44740791942472496</v>
       </c>
     </row>
     <row r="174">
@@ -2506,13 +2518,13 @@
         <v>5</v>
       </c>
       <c r="B174" s="0">
-        <v>4.2999999999999998</v>
+        <v>5.5999999999999996</v>
       </c>
       <c r="C174" s="0">
-        <v>2.0844723232585411</v>
+        <v>4.6042070700865585</v>
       </c>
       <c r="D174" s="0">
-        <v>0.43851140095085955</v>
+        <v>0.43851140095085966</v>
       </c>
     </row>
     <row r="175">
@@ -2520,13 +2532,13 @@
         <v>5.5</v>
       </c>
       <c r="B175" s="0">
-        <v>4.2999999999999998</v>
+        <v>5.5999999999999996</v>
       </c>
       <c r="C175" s="0">
-        <v>2.0377342507780734</v>
+        <v>4.5009714639546488</v>
       </c>
       <c r="D175" s="0">
-        <v>0.42867909115596925</v>
+        <v>0.42867909115596942</v>
       </c>
     </row>
     <row r="176">
@@ -2534,10 +2546,10 @@
         <v>6</v>
       </c>
       <c r="B176" s="0">
-        <v>4.2999999999999998</v>
+        <v>5.5999999999999996</v>
       </c>
       <c r="C176" s="0">
-        <v>1.9903328883393014</v>
+        <v>4.3962707751341989</v>
       </c>
       <c r="D176" s="0">
         <v>0.41870724474761223</v>
@@ -2548,13 +2560,13 @@
         <v>6.5</v>
       </c>
       <c r="B177" s="0">
-        <v>4.2999999999999998</v>
+        <v>5.5999999999999996</v>
       </c>
       <c r="C177" s="0">
-        <v>1.9433784340009257</v>
+        <v>4.2925572222006432</v>
       </c>
       <c r="D177" s="0">
-        <v>0.40882941460179528</v>
+        <v>0.40882941460179523</v>
       </c>
     </row>
     <row r="178">
@@ -2562,13 +2574,13 @@
         <v>7</v>
       </c>
       <c r="B178" s="0">
-        <v>4.2999999999999998</v>
+        <v>5.5999999999999996</v>
       </c>
       <c r="C178" s="0">
-        <v>1.8953113209313144</v>
+        <v>4.1863860155291208</v>
       </c>
       <c r="D178" s="0">
-        <v>0.39871751392715904</v>
+        <v>0.39871751392715915</v>
       </c>
     </row>
     <row r="179">
@@ -2576,13 +2588,13 @@
         <v>7.5</v>
       </c>
       <c r="B179" s="0">
-        <v>4.2999999999999998</v>
+        <v>5.5999999999999996</v>
       </c>
       <c r="C179" s="0">
-        <v>1.9206851977600137</v>
+        <v>4.2424321341494782</v>
       </c>
       <c r="D179" s="0">
-        <v>0.404055428060897</v>
+        <v>0.40405542806089706</v>
       </c>
     </row>
     <row r="180">
@@ -2590,13 +2602,13 @@
         <v>8</v>
       </c>
       <c r="B180" s="0">
-        <v>4.2999999999999998</v>
+        <v>5.5999999999999996</v>
       </c>
       <c r="C180" s="0">
-        <v>1.8730095508729316</v>
+        <v>4.1371256026022962</v>
       </c>
       <c r="D180" s="0">
-        <v>0.39402588030705055</v>
+        <v>0.3940258803070506</v>
       </c>
     </row>
     <row r="181">
@@ -2604,13 +2616,13 @@
         <v>8.5</v>
       </c>
       <c r="B181" s="0">
-        <v>4.2999999999999998</v>
+        <v>5.5999999999999996</v>
       </c>
       <c r="C181" s="0">
-        <v>1.8250543058870312</v>
+        <v>4.0312014914744223</v>
       </c>
       <c r="D181" s="0">
-        <v>0.38393751337261434</v>
+        <v>0.38393751337261439</v>
       </c>
     </row>
     <row r="182">
@@ -2618,13 +2630,13 @@
         <v>9</v>
       </c>
       <c r="B182" s="0">
-        <v>4.2999999999999998</v>
+        <v>5.5999999999999996</v>
       </c>
       <c r="C182" s="0">
-        <v>1.7764369699516571</v>
+        <v>3.9238149460428677</v>
       </c>
       <c r="D182" s="0">
-        <v>0.37370986206075035</v>
+        <v>0.37370986206075046</v>
       </c>
     </row>
     <row r="183">
@@ -2632,10 +2644,10 @@
         <v>9.5</v>
       </c>
       <c r="B183" s="0">
-        <v>4.2999999999999998</v>
+        <v>5.5999999999999996</v>
       </c>
       <c r="C183" s="0">
-        <v>1.7265546662553335</v>
+        <v>3.813634324890848</v>
       </c>
       <c r="D183" s="0">
         <v>0.36321609889946416</v>
@@ -2646,13 +2658,13 @@
         <v>10</v>
       </c>
       <c r="B184" s="0">
-        <v>4.4000000000000004</v>
+        <v>5.7999999999999998</v>
       </c>
       <c r="C184" s="0">
-        <v>1.7956050964865626</v>
+        <v>4.1127923270295632</v>
       </c>
       <c r="D184" s="0">
-        <v>0.35256802490180739</v>
+        <v>0.35256802490180761</v>
       </c>
     </row>
     <row r="185">
@@ -2660,13 +2672,13 @@
         <v>4</v>
       </c>
       <c r="B185" s="0">
-        <v>4.4000000000000004</v>
+        <v>5.7999999999999998</v>
       </c>
       <c r="C185" s="0">
-        <v>2.3102462368702921</v>
+        <v>5.2915660660245623</v>
       </c>
       <c r="D185" s="0">
-        <v>0.45361808916891061</v>
+        <v>0.45361808916891072</v>
       </c>
     </row>
     <row r="186">
@@ -2674,13 +2686,13 @@
         <v>4.5</v>
       </c>
       <c r="B186" s="0">
-        <v>4.4000000000000004</v>
+        <v>5.7999999999999998</v>
       </c>
       <c r="C186" s="0">
-        <v>2.2786182625359421</v>
+        <v>5.2191229155699741</v>
       </c>
       <c r="D186" s="0">
-        <v>0.44740791942472474</v>
+        <v>0.44740791942472485</v>
       </c>
     </row>
     <row r="187">
@@ -2688,13 +2700,13 @@
         <v>5</v>
       </c>
       <c r="B187" s="0">
-        <v>4.4000000000000004</v>
+        <v>5.7999999999999998</v>
       </c>
       <c r="C187" s="0">
-        <v>2.2333088958765335</v>
+        <v>5.1153428495053319</v>
       </c>
       <c r="D187" s="0">
-        <v>0.43851140095085939</v>
+        <v>0.43851140095085955</v>
       </c>
     </row>
     <row r="188">
@@ -2702,13 +2714,13 @@
         <v>5.5</v>
       </c>
       <c r="B188" s="0">
-        <v>4.4000000000000004</v>
+        <v>5.7999999999999998</v>
       </c>
       <c r="C188" s="0">
-        <v>2.183233607333686</v>
+        <v>5.0006465485782563</v>
       </c>
       <c r="D188" s="0">
-        <v>0.42867909115596903</v>
+        <v>0.42867909115596925</v>
       </c>
     </row>
     <row r="189">
@@ -2716,13 +2728,13 @@
         <v>6</v>
       </c>
       <c r="B189" s="0">
-        <v>4.4000000000000004</v>
+        <v>5.7999999999999998</v>
       </c>
       <c r="C189" s="0">
-        <v>2.1324476682593358</v>
+        <v>4.8843225188934021</v>
       </c>
       <c r="D189" s="0">
-        <v>0.41870724474761201</v>
+        <v>0.41870724474761217</v>
       </c>
     </row>
     <row r="190">
@@ -2730,13 +2742,13 @@
         <v>6.5</v>
       </c>
       <c r="B190" s="0">
-        <v>4.4000000000000004</v>
+        <v>5.7999999999999998</v>
       </c>
       <c r="C190" s="0">
-        <v>2.0821405476490726</v>
+        <v>4.7690952119283647</v>
       </c>
       <c r="D190" s="0">
-        <v>0.40882941460179506</v>
+        <v>0.40882941460179517</v>
       </c>
     </row>
     <row r="191">
@@ -2744,10 +2756,10 @@
         <v>7</v>
       </c>
       <c r="B191" s="0">
-        <v>4.4000000000000004</v>
+        <v>5.7999999999999998</v>
       </c>
       <c r="C191" s="0">
-        <v>2.0306413216724706</v>
+        <v>4.6511374149389431</v>
       </c>
       <c r="D191" s="0">
         <v>0.39871751392715898</v>
@@ -2758,13 +2770,13 @@
         <v>7.5</v>
       </c>
       <c r="B192" s="0">
-        <v>4.4000000000000004</v>
+        <v>5.7999999999999998</v>
       </c>
       <c r="C192" s="0">
-        <v>2.0578269571985981</v>
+        <v>4.7134054901499454</v>
       </c>
       <c r="D192" s="0">
-        <v>0.40405542806089673</v>
+        <v>0.404055428060897</v>
       </c>
     </row>
     <row r="193">
@@ -2772,13 +2784,13 @@
         <v>8</v>
       </c>
       <c r="B193" s="0">
-        <v>4.4000000000000004</v>
+        <v>5.7999999999999998</v>
       </c>
       <c r="C193" s="0">
-        <v>2.0067471490756761</v>
+        <v>4.5964083601433758</v>
       </c>
       <c r="D193" s="0">
-        <v>0.39402588030705038</v>
+        <v>0.39402588030705055</v>
       </c>
     </row>
     <row r="194">
@@ -2786,13 +2798,13 @@
         <v>8.5</v>
       </c>
       <c r="B194" s="0">
-        <v>4.4000000000000004</v>
+        <v>5.7999999999999998</v>
       </c>
       <c r="C194" s="0">
-        <v>1.9553677788456472</v>
+        <v>4.478725089994974</v>
       </c>
       <c r="D194" s="0">
-        <v>0.38393751337261423</v>
+        <v>0.38393751337261434</v>
       </c>
     </row>
     <row r="195">
@@ -2800,13 +2812,13 @@
         <v>9</v>
       </c>
       <c r="B195" s="0">
-        <v>4.4000000000000004</v>
+        <v>5.7999999999999998</v>
       </c>
       <c r="C195" s="0">
-        <v>1.9032790427051951</v>
+        <v>4.3594170334839415</v>
       </c>
       <c r="D195" s="0">
-        <v>0.37370986206075019</v>
+        <v>0.37370986206075041</v>
       </c>
     </row>
     <row r="196">
@@ -2814,13 +2826,13 @@
         <v>9.5</v>
       </c>
       <c r="B196" s="0">
-        <v>4.4000000000000004</v>
+        <v>5.7999999999999998</v>
       </c>
       <c r="C196" s="0">
-        <v>1.8498350169204512</v>
+        <v>4.2370047170992562</v>
       </c>
       <c r="D196" s="0">
-        <v>0.36321609889946399</v>
+        <v>0.3632160988994641</v>
       </c>
     </row>
     <row r="197">
@@ -2828,13 +2840,13 @@
         <v>10</v>
       </c>
       <c r="B197" s="0">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="C197" s="0">
-        <v>1.9208362417512452</v>
+        <v>4.5530933137807317</v>
       </c>
       <c r="D197" s="0">
-        <v>0.35256802490180755</v>
+        <v>0.35256802490180772</v>
       </c>
     </row>
     <row r="198">
@@ -2842,13 +2854,13 @@
         <v>4</v>
       </c>
       <c r="B198" s="0">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="C198" s="0">
-        <v>2.4713700734269977</v>
+        <v>5.8580623962714045</v>
       </c>
       <c r="D198" s="0">
-        <v>0.45361808916891072</v>
+        <v>0.45361808916891094</v>
       </c>
     </row>
     <row r="199">
@@ -2856,13 +2868,13 @@
         <v>4.5</v>
       </c>
       <c r="B199" s="0">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="C199" s="0">
-        <v>2.4375362647162349</v>
+        <v>5.7778637385866336</v>
       </c>
       <c r="D199" s="0">
-        <v>0.44740791942472485</v>
+        <v>0.44740791942472508</v>
       </c>
     </row>
     <row r="200">
@@ -2870,13 +2882,13 @@
         <v>5</v>
       </c>
       <c r="B200" s="0">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="C200" s="0">
-        <v>2.3890668803619124</v>
+        <v>5.6629733460430538</v>
       </c>
       <c r="D200" s="0">
-        <v>0.43851140095085955</v>
+        <v>0.43851140095085972</v>
       </c>
     </row>
     <row r="201">
@@ -2884,13 +2896,13 @@
         <v>5.5</v>
       </c>
       <c r="B201" s="0">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="C201" s="0">
-        <v>2.3354991837467387</v>
+        <v>5.5359980651774583</v>
       </c>
       <c r="D201" s="0">
-        <v>0.42867909115596925</v>
+        <v>0.42867909115596953</v>
       </c>
     </row>
     <row r="202">
@@ -2898,13 +2910,13 @@
         <v>6</v>
       </c>
       <c r="B202" s="0">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="C202" s="0">
-        <v>2.2811712735975305</v>
+        <v>5.40722079667563</v>
       </c>
       <c r="D202" s="0">
-        <v>0.41870724474761217</v>
+        <v>0.41870724474761234</v>
       </c>
     </row>
     <row r="203">
@@ -2912,13 +2924,13 @@
         <v>6.5</v>
       </c>
       <c r="B203" s="0">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="C203" s="0">
-        <v>2.2273555762176205</v>
+        <v>5.2796576621454729</v>
       </c>
       <c r="D203" s="0">
-        <v>0.40882941460179523</v>
+        <v>0.40882941460179539</v>
       </c>
     </row>
     <row r="204">
@@ -2926,13 +2938,13 @@
         <v>7</v>
       </c>
       <c r="B204" s="0">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="C204" s="0">
-        <v>2.1722646322948429</v>
+        <v>5.1490717209951855</v>
       </c>
       <c r="D204" s="0">
-        <v>0.3987175139271591</v>
+        <v>0.39871751392715926</v>
       </c>
     </row>
     <row r="205">
@@ -2940,13 +2952,13 @@
         <v>7.5</v>
       </c>
       <c r="B205" s="0">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="C205" s="0">
-        <v>2.2013462795210641</v>
+        <v>5.2180059959017839</v>
       </c>
       <c r="D205" s="0">
-        <v>0.40405542806089695</v>
+        <v>0.40405542806089717</v>
       </c>
     </row>
     <row r="206">
@@ -2954,13 +2966,13 @@
         <v>8</v>
       </c>
       <c r="B206" s="0">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="C206" s="0">
-        <v>2.1467040049718382</v>
+        <v>5.0884835673406545</v>
       </c>
       <c r="D206" s="0">
-        <v>0.3940258803070506</v>
+        <v>0.39402588030705071</v>
       </c>
     </row>
     <row r="207">
@@ -2968,13 +2980,13 @@
         <v>8.5</v>
       </c>
       <c r="B207" s="0">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="C207" s="0">
-        <v>2.091741275912256</v>
+        <v>4.9582015429031285</v>
       </c>
       <c r="D207" s="0">
-        <v>0.38393751337261434</v>
+        <v>0.38393751337261461</v>
       </c>
     </row>
     <row r="208">
@@ -2982,13 +2994,13 @@
         <v>9</v>
       </c>
       <c r="B208" s="0">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="C208" s="0">
-        <v>2.0360197075332329</v>
+        <v>4.826120788226925</v>
       </c>
       <c r="D208" s="0">
-        <v>0.3737098620607503</v>
+        <v>0.37370986206075046</v>
       </c>
     </row>
     <row r="209">
@@ -2996,13 +3008,13 @@
         <v>9.5</v>
       </c>
       <c r="B209" s="0">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="C209" s="0">
-        <v>1.9788483273487525</v>
+        <v>4.6906034426044529</v>
       </c>
       <c r="D209" s="0">
-        <v>0.3632160988994641</v>
+        <v>0.36321609889946432</v>
       </c>
     </row>
     <row r="210">
@@ -3010,13 +3022,13 @@
         <v>10</v>
       </c>
       <c r="B210" s="0">
-        <v>4.5999999999999996</v>
+        <v>6.2000000000000002</v>
       </c>
       <c r="C210" s="0">
-        <v>2.0517587536581541</v>
+        <v>5.0237482559571021</v>
       </c>
       <c r="D210" s="0">
-        <v>0.35256802490180783</v>
+        <v>0.35256802490180766</v>
       </c>
     </row>
     <row r="211">
@@ -3024,13 +3036,13 @@
         <v>4</v>
       </c>
       <c r="B211" s="0">
-        <v>4.5999999999999996</v>
+        <v>6.2000000000000002</v>
       </c>
       <c r="C211" s="0">
-        <v>2.6398164879790431</v>
+        <v>6.4636124758267162</v>
       </c>
       <c r="D211" s="0">
-        <v>0.45361808916891094</v>
+        <v>0.45361808916891067</v>
       </c>
     </row>
     <row r="212">
@@ -3038,13 +3050,13 @@
         <v>4.5</v>
       </c>
       <c r="B212" s="0">
-        <v>4.5999999999999996</v>
+        <v>6.2000000000000002</v>
       </c>
       <c r="C212" s="0">
-        <v>2.6036765965697612</v>
+        <v>6.3751236531938646</v>
       </c>
       <c r="D212" s="0">
-        <v>0.44740791942472508</v>
+        <v>0.44740791942472491</v>
       </c>
     </row>
     <row r="213">
@@ -3052,13 +3064,13 @@
         <v>5</v>
       </c>
       <c r="B213" s="0">
-        <v>4.5999999999999996</v>
+        <v>6.2000000000000002</v>
       </c>
       <c r="C213" s="0">
-        <v>2.5519035815298454</v>
+        <v>6.2483569982210589</v>
       </c>
       <c r="D213" s="0">
-        <v>0.43851140095085972</v>
+        <v>0.43851140095085961</v>
       </c>
     </row>
     <row r="214">
@@ -3066,13 +3078,13 @@
         <v>5.5</v>
       </c>
       <c r="B214" s="0">
-        <v>4.5999999999999996</v>
+        <v>6.2000000000000002</v>
       </c>
       <c r="C214" s="0">
-        <v>2.4946847577412639</v>
+        <v>6.1082562355445047</v>
       </c>
       <c r="D214" s="0">
-        <v>0.42867909115596953</v>
+        <v>0.42867909115596936</v>
       </c>
     </row>
     <row r="215">
@@ -3080,13 +3092,13 @@
         <v>6</v>
       </c>
       <c r="B215" s="0">
-        <v>4.5999999999999996</v>
+        <v>6.2000000000000002</v>
       </c>
       <c r="C215" s="0">
-        <v>2.4366539049315694</v>
+        <v>5.9661672131023575</v>
       </c>
       <c r="D215" s="0">
-        <v>0.41870724474761234</v>
+        <v>0.41870724474761223</v>
       </c>
     </row>
     <row r="216">
@@ -3094,13 +3106,13 @@
         <v>6.5</v>
       </c>
       <c r="B216" s="0">
-        <v>4.5999999999999996</v>
+        <v>6.2000000000000002</v>
       </c>
       <c r="C216" s="0">
-        <v>2.3791701768638505</v>
+        <v>5.8254178301102124</v>
       </c>
       <c r="D216" s="0">
-        <v>0.40882941460179539</v>
+        <v>0.40882941460179517</v>
       </c>
     </row>
     <row r="217">
@@ -3108,13 +3120,13 @@
         <v>7</v>
       </c>
       <c r="B217" s="0">
-        <v>4.5999999999999996</v>
+        <v>6.2000000000000002</v>
       </c>
       <c r="C217" s="0">
-        <v>2.3203242825684596</v>
+        <v>5.6813331718580562</v>
       </c>
       <c r="D217" s="0">
-        <v>0.39871751392715926</v>
+        <v>0.3987175139271591</v>
       </c>
     </row>
     <row r="218">
@@ -3122,13 +3134,13 @@
         <v>7.5</v>
       </c>
       <c r="B218" s="0">
-        <v>4.5999999999999996</v>
+        <v>6.2000000000000002</v>
       </c>
       <c r="C218" s="0">
-        <v>2.3513881093384077</v>
+        <v>5.7573932082929637</v>
       </c>
       <c r="D218" s="0">
-        <v>0.40405542806089728</v>
+        <v>0.40405542806089706</v>
       </c>
     </row>
     <row r="219">
@@ -3136,13 +3148,13 @@
         <v>8</v>
       </c>
       <c r="B219" s="0">
-        <v>4.5999999999999996</v>
+        <v>6.2000000000000002</v>
       </c>
       <c r="C219" s="0">
-        <v>2.2930214653271759</v>
+        <v>5.6144819983201995</v>
       </c>
       <c r="D219" s="0">
-        <v>0.39402588030705082</v>
+        <v>0.39402588030705049</v>
       </c>
     </row>
     <row r="220">
@@ -3150,13 +3162,13 @@
         <v>8.5</v>
       </c>
       <c r="B220" s="0">
-        <v>4.5999999999999996</v>
+        <v>6.2000000000000002</v>
       </c>
       <c r="C220" s="0">
-        <v>2.2343125249074944</v>
+        <v>5.4707326727639645</v>
       </c>
       <c r="D220" s="0">
-        <v>0.38393751337261461</v>
+        <v>0.38393751337261439</v>
       </c>
     </row>
     <row r="221">
@@ -3164,13 +3176,13 @@
         <v>9</v>
       </c>
       <c r="B221" s="0">
-        <v>4.5999999999999996</v>
+        <v>6.2000000000000002</v>
       </c>
       <c r="C221" s="0">
-        <v>2.1747930233465556</v>
+        <v>5.3249986815580845</v>
       </c>
       <c r="D221" s="0">
-        <v>0.37370986206075058</v>
+        <v>0.3737098620607503</v>
       </c>
     </row>
     <row r="222">
@@ -3178,13 +3190,13 @@
         <v>9.5</v>
       </c>
       <c r="B222" s="0">
-        <v>4.5999999999999996</v>
+        <v>6.2000000000000002</v>
       </c>
       <c r="C222" s="0">
-        <v>2.11372489208031</v>
+        <v>5.1754728577270077</v>
       </c>
       <c r="D222" s="0">
-        <v>0.36321609889946432</v>
+        <v>0.36321609889946416</v>
       </c>
     </row>
     <row r="223">
@@ -3192,10 +3204,10 @@
         <v>10</v>
       </c>
       <c r="B223" s="0">
-        <v>4.7000000000000002</v>
+        <v>6.4000000000000004</v>
       </c>
       <c r="C223" s="0">
-        <v>2.1884991070215594</v>
+        <v>5.5257689520728519</v>
       </c>
       <c r="D223" s="0">
         <v>0.35256802490180766</v>
@@ -3206,13 +3218,13 @@
         <v>4</v>
       </c>
       <c r="B224" s="0">
-        <v>4.7000000000000002</v>
+        <v>6.4000000000000004</v>
       </c>
       <c r="C224" s="0">
-        <v>2.8157482044818796</v>
+        <v>7.1095180963341225</v>
       </c>
       <c r="D224" s="0">
-        <v>0.45361808916891089</v>
+        <v>0.45361808916891067</v>
       </c>
     </row>
     <row r="225">
@@ -3220,10 +3232,10 @@
         <v>4.5</v>
       </c>
       <c r="B225" s="0">
-        <v>4.7000000000000002</v>
+        <v>6.4000000000000004</v>
       </c>
       <c r="C225" s="0">
-        <v>2.7771997543114808</v>
+        <v>7.0121866291113619</v>
       </c>
       <c r="D225" s="0">
         <v>0.44740791942472491</v>
@@ -3234,10 +3246,10 @@
         <v>5</v>
       </c>
       <c r="B226" s="0">
-        <v>4.7000000000000002</v>
+        <v>6.4000000000000004</v>
       </c>
       <c r="C226" s="0">
-        <v>2.7219763041954996</v>
+        <v>6.8727522445606963</v>
       </c>
       <c r="D226" s="0">
         <v>0.43851140095085966</v>
@@ -3248,13 +3260,13 @@
         <v>5.5</v>
       </c>
       <c r="B227" s="0">
-        <v>4.7000000000000002</v>
+        <v>6.4000000000000004</v>
       </c>
       <c r="C227" s="0">
-        <v>2.6609441070412925</v>
+        <v>6.7186512814716632</v>
       </c>
       <c r="D227" s="0">
-        <v>0.42867909115596942</v>
+        <v>0.42867909115596931</v>
       </c>
     </row>
     <row r="228">
@@ -3262,13 +3274,13 @@
         <v>6</v>
       </c>
       <c r="B228" s="0">
-        <v>4.7000000000000002</v>
+        <v>6.4000000000000004</v>
       </c>
       <c r="C228" s="0">
-        <v>2.5990457628391379</v>
+        <v>6.5623633727950725</v>
       </c>
       <c r="D228" s="0">
-        <v>0.41870724474761223</v>
+        <v>0.41870724474761206</v>
       </c>
     </row>
     <row r="229">
@@ -3276,13 +3288,13 @@
         <v>6.5</v>
       </c>
       <c r="B229" s="0">
-        <v>4.7000000000000002</v>
+        <v>6.4000000000000004</v>
       </c>
       <c r="C229" s="0">
-        <v>2.5377310067450427</v>
+        <v>6.4075489730808437</v>
       </c>
       <c r="D229" s="0">
-        <v>0.40882941460179517</v>
+        <v>0.40882941460179512</v>
       </c>
     </row>
     <row r="230">
@@ -3290,13 +3302,13 @@
         <v>7</v>
       </c>
       <c r="B230" s="0">
-        <v>4.7000000000000002</v>
+        <v>6.4000000000000004</v>
       </c>
       <c r="C230" s="0">
-        <v>2.474963302263347</v>
+        <v>6.2490660056877845</v>
       </c>
       <c r="D230" s="0">
-        <v>0.3987175139271591</v>
+        <v>0.39871751392715904</v>
       </c>
     </row>
     <row r="231">
@@ -3304,13 +3316,13 @@
         <v>7.5</v>
       </c>
       <c r="B231" s="0">
-        <v>4.7000000000000002</v>
+        <v>6.4000000000000004</v>
       </c>
       <c r="C231" s="0">
-        <v>2.5080973912616242</v>
+        <v>6.3327266842114662</v>
       </c>
       <c r="D231" s="0">
-        <v>0.40405542806089706</v>
+        <v>0.40405542806089689</v>
       </c>
     </row>
     <row r="232">
@@ -3318,13 +3330,13 @@
         <v>8</v>
       </c>
       <c r="B232" s="0">
-        <v>4.7000000000000002</v>
+        <v>6.4000000000000004</v>
       </c>
       <c r="C232" s="0">
-        <v>2.445840876907448</v>
+        <v>6.1755344272080936</v>
       </c>
       <c r="D232" s="0">
-        <v>0.39402588030705066</v>
+        <v>0.39402588030705055</v>
       </c>
     </row>
     <row r="233">
@@ -3332,13 +3344,13 @@
         <v>8.5</v>
       </c>
       <c r="B233" s="0">
-        <v>4.7000000000000002</v>
+        <v>6.4000000000000004</v>
       </c>
       <c r="C233" s="0">
-        <v>2.3832192536519967</v>
+        <v>6.0174203021425789</v>
       </c>
       <c r="D233" s="0">
-        <v>0.38393751337261439</v>
+        <v>0.38393751337261434</v>
       </c>
     </row>
     <row r="234">
@@ -3346,13 +3358,13 @@
         <v>9</v>
       </c>
       <c r="B234" s="0">
-        <v>4.7000000000000002</v>
+        <v>6.4000000000000004</v>
       </c>
       <c r="C234" s="0">
-        <v>2.3197330490559445</v>
+        <v>5.8571231847636982</v>
       </c>
       <c r="D234" s="0">
-        <v>0.37370986206075041</v>
+        <v>0.37370986206075035</v>
       </c>
     </row>
     <row r="235">
@@ -3360,13 +3372,13 @@
         <v>9.5</v>
       </c>
       <c r="B235" s="0">
-        <v>4.7000000000000002</v>
+        <v>6.4000000000000004</v>
       </c>
       <c r="C235" s="0">
-        <v>2.2545950056551938</v>
+        <v>5.6926553187875069</v>
       </c>
       <c r="D235" s="0">
-        <v>0.3632160988994641</v>
+        <v>0.36321609889946416</v>
       </c>
     </row>
     <row r="236">
@@ -3374,13 +3386,13 @@
         <v>10</v>
       </c>
       <c r="B236" s="0">
-        <v>4.7999999999999998</v>
+        <v>6.5999999999999996</v>
       </c>
       <c r="C236" s="0">
-        <v>2.3311837766557346</v>
+        <v>6.0601672006421516</v>
       </c>
       <c r="D236" s="0">
-        <v>0.35256802490180777</v>
+        <v>0.35256802490180761</v>
       </c>
     </row>
     <row r="237">
@@ -3388,13 +3400,13 @@
         <v>4</v>
       </c>
       <c r="B237" s="0">
-        <v>4.7999999999999998</v>
+        <v>6.5999999999999996</v>
       </c>
       <c r="C237" s="0">
-        <v>2.9993279468909586</v>
+        <v>7.7970810494372351</v>
       </c>
       <c r="D237" s="0">
-        <v>0.45361808916891089</v>
+        <v>0.45361808916891067</v>
       </c>
     </row>
     <row r="238">
@@ -3402,13 +3414,13 @@
         <v>4.5</v>
       </c>
       <c r="B238" s="0">
-        <v>4.7999999999999998</v>
+        <v>6.5999999999999996</v>
       </c>
       <c r="C238" s="0">
-        <v>2.9582662341563566</v>
+        <v>7.690336636058805</v>
       </c>
       <c r="D238" s="0">
-        <v>0.44740791942472519</v>
+        <v>0.44740791942472485</v>
       </c>
     </row>
     <row r="239">
@@ -3416,13 +3428,13 @@
         <v>5</v>
       </c>
       <c r="B239" s="0">
-        <v>4.7999999999999998</v>
+        <v>6.5999999999999996</v>
       </c>
       <c r="C239" s="0">
-        <v>2.8994423531740434</v>
+        <v>7.5374175235833025</v>
       </c>
       <c r="D239" s="0">
-        <v>0.43851140095085972</v>
+        <v>0.43851140095085961</v>
       </c>
     </row>
     <row r="240">
@@ -3430,13 +3442,13 @@
         <v>5.5</v>
       </c>
       <c r="B240" s="0">
-        <v>4.7999999999999998</v>
+        <v>6.5999999999999996</v>
       </c>
       <c r="C240" s="0">
-        <v>2.8344310093708582</v>
+        <v>7.3684134247511945</v>
       </c>
       <c r="D240" s="0">
-        <v>0.42867909115596953</v>
+        <v>0.42867909115596936</v>
       </c>
     </row>
     <row r="241">
@@ -3444,13 +3456,13 @@
         <v>6</v>
       </c>
       <c r="B241" s="0">
-        <v>4.7999999999999998</v>
+        <v>6.5999999999999996</v>
       </c>
       <c r="C241" s="0">
-        <v>2.7684970478979229</v>
+        <v>7.1970108803752604</v>
       </c>
       <c r="D241" s="0">
-        <v>0.41870724474761245</v>
+        <v>0.41870724474761217</v>
       </c>
     </row>
     <row r="242">
@@ -3458,13 +3470,13 @@
         <v>6.5</v>
       </c>
       <c r="B242" s="0">
-        <v>4.7999999999999998</v>
+        <v>6.5999999999999996</v>
       </c>
       <c r="C242" s="0">
-        <v>2.7031847230184822</v>
+        <v>7.027224348315622</v>
       </c>
       <c r="D242" s="0">
-        <v>0.40882941460179545</v>
+        <v>0.40882941460179523</v>
       </c>
     </row>
     <row r="243">
@@ -3472,13 +3484,13 @@
         <v>7</v>
       </c>
       <c r="B243" s="0">
-        <v>4.7999999999999998</v>
+        <v>6.5999999999999996</v>
       </c>
       <c r="C243" s="0">
-        <v>2.6363247211495349</v>
+        <v>6.853414460644589</v>
       </c>
       <c r="D243" s="0">
-        <v>0.39871751392715932</v>
+        <v>0.3987175139271591</v>
       </c>
     </row>
     <row r="244">
@@ -3486,13 +3498,13 @@
         <v>7.5</v>
       </c>
       <c r="B244" s="0">
-        <v>4.7999999999999998</v>
+        <v>6.5999999999999996</v>
       </c>
       <c r="C244" s="0">
-        <v>2.6716190699017131</v>
+        <v>6.9451659805452719</v>
       </c>
       <c r="D244" s="0">
-        <v>0.40405542806089717</v>
+        <v>0.404055428060897</v>
       </c>
     </row>
     <row r="245">
@@ -3500,13 +3512,13 @@
         <v>8</v>
       </c>
       <c r="B245" s="0">
-        <v>4.7999999999999998</v>
+        <v>6.5999999999999996</v>
       </c>
       <c r="C245" s="0">
-        <v>2.6053035864784158</v>
+        <v>6.7727716281304104</v>
       </c>
       <c r="D245" s="0">
-        <v>0.39402588030705082</v>
+        <v>0.39402588030705066</v>
       </c>
     </row>
     <row r="246">
@@ -3514,13 +3526,13 @@
         <v>8.5</v>
       </c>
       <c r="B246" s="0">
-        <v>4.7999999999999998</v>
+        <v>6.5999999999999996</v>
       </c>
       <c r="C246" s="0">
-        <v>2.5385991899664013</v>
+        <v>6.5993662536040603</v>
       </c>
       <c r="D246" s="0">
-        <v>0.38393751337261456</v>
+        <v>0.38393751337261439</v>
       </c>
     </row>
     <row r="247">
@@ -3528,13 +3540,13 @@
         <v>9</v>
       </c>
       <c r="B247" s="0">
-        <v>4.7999999999999998</v>
+        <v>6.5999999999999996</v>
       </c>
       <c r="C247" s="0">
-        <v>2.4709738435721857</v>
+        <v>6.4235667691300353</v>
       </c>
       <c r="D247" s="0">
-        <v>0.37370986206075052</v>
+        <v>0.37370986206075035</v>
       </c>
     </row>
     <row r="248">
@@ -3542,13 +3554,13 @@
         <v>9.5</v>
       </c>
       <c r="B248" s="0">
-        <v>4.7999999999999998</v>
+        <v>6.5999999999999996</v>
       </c>
       <c r="C248" s="0">
-        <v>2.4015889626134799</v>
+        <v>6.2431931821065234</v>
       </c>
       <c r="D248" s="0">
-        <v>0.36321609889946432</v>
+        <v>0.3632160988994641</v>
       </c>
     </row>
     <row r="249">
@@ -3556,13 +3568,13 @@
         <v>10</v>
       </c>
       <c r="B249" s="0">
-        <v>4.9000000000000004</v>
+        <v>6.7999999999999998</v>
       </c>
       <c r="C249" s="0">
-        <v>2.4799392373749503</v>
+        <v>6.627954800179177</v>
       </c>
       <c r="D249" s="0">
-        <v>0.35256802490180761</v>
+        <v>0.35256802490180755</v>
       </c>
     </row>
     <row r="250">
@@ -3570,13 +3582,13 @@
         <v>4</v>
       </c>
       <c r="B250" s="0">
-        <v>4.9000000000000004</v>
+        <v>6.7999999999999998</v>
       </c>
       <c r="C250" s="0">
-        <v>3.1907184391617331</v>
+        <v>8.5276031267796739</v>
       </c>
       <c r="D250" s="0">
-        <v>0.45361808916891072</v>
+        <v>0.45361808916891078</v>
       </c>
     </row>
     <row r="251">
@@ -3584,13 +3596,13 @@
         <v>4.5</v>
       </c>
       <c r="B251" s="0">
-        <v>4.9000000000000004</v>
+        <v>6.7999999999999998</v>
       </c>
       <c r="C251" s="0">
-        <v>3.1470365323193463</v>
+        <v>8.410857643755886</v>
       </c>
       <c r="D251" s="0">
-        <v>0.44740791942472496</v>
+        <v>0.44740791942472491</v>
       </c>
     </row>
     <row r="252">
@@ -3598,13 +3610,13 @@
         <v>5</v>
       </c>
       <c r="B252" s="0">
-        <v>4.9000000000000004</v>
+        <v>6.7999999999999998</v>
       </c>
       <c r="C252" s="0">
-        <v>3.0844590332806447</v>
+        <v>8.2436112738102274</v>
       </c>
       <c r="D252" s="0">
-        <v>0.43851140095085961</v>
+        <v>0.43851140095085966</v>
       </c>
     </row>
     <row r="253">
@@ -3612,10 +3624,10 @@
         <v>5.5</v>
       </c>
       <c r="B253" s="0">
-        <v>4.9000000000000004</v>
+        <v>6.7999999999999998</v>
       </c>
       <c r="C253" s="0">
-        <v>3.0152992424539935</v>
+        <v>8.0587728871753583</v>
       </c>
       <c r="D253" s="0">
         <v>0.42867909115596925</v>
@@ -3626,13 +3638,13 @@
         <v>6</v>
       </c>
       <c r="B254" s="0">
-        <v>4.9000000000000004</v>
+        <v>6.7999999999999998</v>
       </c>
       <c r="C254" s="0">
-        <v>2.9451579606856071</v>
+        <v>7.8713113404644037</v>
       </c>
       <c r="D254" s="0">
-        <v>0.41870724474761217</v>
+        <v>0.41870724474761228</v>
       </c>
     </row>
     <row r="255">
@@ -3640,13 +3652,13 @@
         <v>6.5</v>
       </c>
       <c r="B255" s="0">
-        <v>4.9000000000000004</v>
+        <v>6.7999999999999998</v>
       </c>
       <c r="C255" s="0">
-        <v>2.8756779828414474</v>
+        <v>7.6856172130728</v>
       </c>
       <c r="D255" s="0">
-        <v>0.40882941460179517</v>
+        <v>0.40882941460179528</v>
       </c>
     </row>
     <row r="256">
@@ -3654,13 +3666,13 @@
         <v>7</v>
       </c>
       <c r="B256" s="0">
-        <v>4.9000000000000004</v>
+        <v>6.7999999999999998</v>
       </c>
       <c r="C256" s="0">
-        <v>2.8045515689970486</v>
+        <v>7.4955227748886921</v>
       </c>
       <c r="D256" s="0">
-        <v>0.3987175139271591</v>
+        <v>0.39871751392715915</v>
       </c>
     </row>
     <row r="257">
@@ -3668,13 +3680,13 @@
         <v>7.5</v>
       </c>
       <c r="B257" s="0">
-        <v>4.9000000000000004</v>
+        <v>6.7999999999999998</v>
       </c>
       <c r="C257" s="0">
-        <v>2.8420980898696708</v>
+        <v>7.5958706541823577</v>
       </c>
       <c r="D257" s="0">
-        <v>0.404055428060897</v>
+        <v>0.40405542806089706</v>
       </c>
     </row>
     <row r="258">
@@ -3682,13 +3694,13 @@
         <v>8</v>
       </c>
       <c r="B258" s="0">
-        <v>4.9000000000000004</v>
+        <v>6.7999999999999998</v>
       </c>
       <c r="C258" s="0">
-        <v>2.7715509408058359</v>
+        <v>7.4073243752132241</v>
       </c>
       <c r="D258" s="0">
-        <v>0.39402588030705049</v>
+        <v>0.39402588030705066</v>
       </c>
     </row>
     <row r="259">
@@ -3696,10 +3708,10 @@
         <v>8.5</v>
       </c>
       <c r="B259" s="0">
-        <v>4.9000000000000004</v>
+        <v>6.7999999999999998</v>
       </c>
       <c r="C259" s="0">
-        <v>2.7005900616713427</v>
+        <v>7.2176723497134985</v>
       </c>
       <c r="D259" s="0">
         <v>0.38393751337261439</v>
@@ -3710,10 +3722,10 @@
         <v>9</v>
       </c>
       <c r="B260" s="0">
-        <v>4.9000000000000004</v>
+        <v>6.7999999999999998</v>
       </c>
       <c r="C260" s="0">
-        <v>2.6286494658060624</v>
+        <v>7.0254019059433697</v>
       </c>
       <c r="D260" s="0">
         <v>0.37370986206075035</v>
@@ -3724,13 +3736,13 @@
         <v>9.5</v>
       </c>
       <c r="B261" s="0">
-        <v>4.9000000000000004</v>
+        <v>6.7999999999999998</v>
       </c>
       <c r="C261" s="0">
-        <v>2.5548370574952366</v>
+        <v>6.8281288040046428</v>
       </c>
       <c r="D261" s="0">
-        <v>0.3632160988994641</v>
+        <v>0.36321609889946421</v>
       </c>
     </row>
     <row r="262">
@@ -3738,13 +3750,13 @@
         <v>10</v>
       </c>
       <c r="B262" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C262" s="0">
-        <v>2.6348919639934776</v>
+        <v>7.2301435491981056</v>
       </c>
       <c r="D262" s="0">
-        <v>0.35256802490180755</v>
+        <v>0.35256802490180772</v>
       </c>
     </row>
     <row r="263">
@@ -3752,13 +3764,13 @@
         <v>4</v>
       </c>
       <c r="B263" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C263" s="0">
-        <v>3.3900824052496543</v>
+        <v>9.3023861200050515</v>
       </c>
       <c r="D263" s="0">
-        <v>0.45361808916891078</v>
+        <v>0.45361808916891083</v>
       </c>
     </row>
     <row r="264">
@@ -3766,13 +3778,13 @@
         <v>4.5</v>
       </c>
       <c r="B264" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C264" s="0">
-        <v>3.3436711450154113</v>
+        <v>9.1750336219222905</v>
       </c>
       <c r="D264" s="0">
-        <v>0.44740791942472491</v>
+        <v>0.44740791942472502</v>
       </c>
     </row>
     <row r="265">
@@ -3780,10 +3792,10 @@
         <v>5</v>
       </c>
       <c r="B265" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C265" s="0">
-        <v>3.2771836493304702</v>
+        <v>8.9925919337628102</v>
       </c>
       <c r="D265" s="0">
         <v>0.43851140095085961</v>
@@ -3794,13 +3806,13 @@
         <v>5.5</v>
       </c>
       <c r="B266" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C266" s="0">
-        <v>3.2037025840147311</v>
+        <v>8.7909598905364241</v>
       </c>
       <c r="D266" s="0">
-        <v>0.42867909115596931</v>
+        <v>0.42867909115596942</v>
       </c>
     </row>
     <row r="267">
@@ -3808,10 +3820,10 @@
         <v>6</v>
       </c>
       <c r="B267" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C267" s="0">
-        <v>3.1291787017798773</v>
+        <v>8.5864663576839835</v>
       </c>
       <c r="D267" s="0">
         <v>0.41870724474761223</v>
@@ -3822,13 +3834,13 @@
         <v>6.5</v>
       </c>
       <c r="B268" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C268" s="0">
-        <v>3.0553574433712214</v>
+        <v>8.3839008246106328</v>
       </c>
       <c r="D268" s="0">
-        <v>0.40882941460179523</v>
+        <v>0.40882941460179528</v>
       </c>
     </row>
     <row r="269">
@@ -3836,10 +3848,10 @@
         <v>7</v>
       </c>
       <c r="B269" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C269" s="0">
-        <v>2.979786875575916</v>
+        <v>8.1765351865803133</v>
       </c>
       <c r="D269" s="0">
         <v>0.3987175139271591</v>
@@ -3850,13 +3862,13 @@
         <v>7.5</v>
       </c>
       <c r="B270" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C270" s="0">
-        <v>3.0196793957764942</v>
+        <v>8.2860002620107007</v>
       </c>
       <c r="D270" s="0">
-        <v>0.404055428060897</v>
+        <v>0.40405542806089706</v>
       </c>
     </row>
     <row r="271">
@@ -3864,13 +3876,13 @@
         <v>8</v>
       </c>
       <c r="B271" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C271" s="0">
-        <v>2.9447242866554704</v>
+        <v>8.0803234425826123</v>
       </c>
       <c r="D271" s="0">
-        <v>0.39402588030705055</v>
+        <v>0.39402588030705066</v>
       </c>
     </row>
     <row r="272">
@@ -3878,13 +3890,13 @@
         <v>8.5</v>
       </c>
       <c r="B272" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C272" s="0">
-        <v>2.8693295965874568</v>
+        <v>7.8734404130359836</v>
       </c>
       <c r="D272" s="0">
-        <v>0.38393751337261439</v>
+        <v>0.3839375133726145</v>
       </c>
     </row>
     <row r="273">
@@ -3892,13 +3904,13 @@
         <v>9</v>
       </c>
       <c r="B273" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C273" s="0">
-        <v>2.7928939746683583</v>
+        <v>7.6637010664899767</v>
       </c>
       <c r="D273" s="0">
-        <v>0.37370986206075035</v>
+        <v>0.37370986206075041</v>
       </c>
     </row>
     <row r="274">
@@ -3906,13 +3918,13 @@
         <v>9.5</v>
       </c>
       <c r="B274" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C274" s="0">
-        <v>2.7144695848405385</v>
+        <v>7.4485045408024382</v>
       </c>
       <c r="D274" s="0">
-        <v>0.3632160988994641</v>
+        <v>0.36321609889946416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>